<commit_message>
Update add oscillating pressure gradient
</commit_message>
<xml_diff>
--- a/case_number_20250816.xlsx
+++ b/case_number_20250816.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chang\Nutstore\1\Nutstore\Workspace\convection_time_varying_T\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43378C40-84B0-459D-93F5-B9F6B68EC125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08FB94E-0192-4B93-8DCF-6F9CAE9ED660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1113" yWindow="1480" windowWidth="19200" windowHeight="10060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="47">
   <si>
     <t>omega</t>
   </si>
@@ -142,6 +142,42 @@
   </si>
   <si>
     <t>400G</t>
+  </si>
+  <si>
+    <t>channel-cetner resolved</t>
+  </si>
+  <si>
+    <t>10358563, 10424250, 10439614</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>channel-center unresolved</t>
+  </si>
+  <si>
+    <t>not long enough, not fully turbulent yet, channel center unresolved</t>
+  </si>
+  <si>
+    <t>12h</t>
+  </si>
+  <si>
+    <t>4 node, each 950GB memory</t>
+  </si>
+  <si>
+    <t>omega (dP/dx)</t>
+  </si>
+  <si>
+    <t>A (dP/dx)</t>
+  </si>
+  <si>
+    <t>Below: with oscillating pressure gradient: continue from 10424250, t=100 of fully developed turbulence. 10439614 is the same continuation from 10424250 without oscillation</t>
+  </si>
+  <si>
+    <t>NREL job ID</t>
+  </si>
+  <si>
+    <t>600G</t>
   </si>
 </sst>
 </file>
@@ -157,12 +193,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -177,9 +219,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,18 +669,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0792B6-F3DE-44AA-920E-7B8294731BF8}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="1" max="1" width="31.3515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
       <c r="B1" t="s">
         <v>16</v>
       </c>
@@ -645,40 +691,49 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>25</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="Q1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>10249087</v>
       </c>
@@ -688,37 +743,43 @@
       <c r="C2">
         <v>0.71</v>
       </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2">
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2">
         <v>192</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>129</v>
       </c>
-      <c r="I2">
-        <v>160</v>
-      </c>
-      <c r="J2">
+      <c r="K2">
+        <v>160</v>
+      </c>
+      <c r="L2">
         <v>2E-3</v>
       </c>
-      <c r="K2">
-        <v>96</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2">
+        <v>96</v>
+      </c>
+      <c r="N2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
-      <c r="A3">
-        <v>10358563</v>
+      <c r="Q2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>36</v>
       </c>
       <c r="B3">
         <v>180</v>
@@ -726,42 +787,48 @@
       <c r="C3">
         <v>0.71</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3">
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3">
         <v>192</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <f>129*2</f>
         <v>258</v>
       </c>
-      <c r="I3">
-        <v>160</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1E-4</v>
-      </c>
       <c r="K3">
-        <v>96</v>
-      </c>
-      <c r="L3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" t="s">
+        <v>160</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M3">
+        <v>96</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" t="s">
         <v>34</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="Q3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>10336395</v>
       </c>
@@ -771,41 +838,47 @@
       <c r="C4">
         <v>0.71</v>
       </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>22</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>288</v>
       </c>
-      <c r="H4">
-        <v>180</v>
-      </c>
-      <c r="I4">
+      <c r="J4">
+        <v>180</v>
+      </c>
+      <c r="K4">
         <v>240</v>
       </c>
-      <c r="J4" s="1">
+      <c r="L4" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="K4">
-        <v>96</v>
-      </c>
-      <c r="L4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="M4">
+        <v>96</v>
+      </c>
+      <c r="N4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" t="s">
         <v>26</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="Q4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>10337407</v>
       </c>
@@ -815,38 +888,996 @@
       <c r="C5">
         <v>0.71</v>
       </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5">
         <v>2</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>22</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>288</v>
       </c>
-      <c r="H5">
-        <v>180</v>
-      </c>
-      <c r="I5">
+      <c r="J5">
+        <v>180</v>
+      </c>
+      <c r="K5">
         <v>240</v>
       </c>
-      <c r="J5" s="1">
+      <c r="L5" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="K5">
-        <v>96</v>
-      </c>
-      <c r="L5" t="s">
-        <v>28</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="M5">
+        <v>96</v>
+      </c>
+      <c r="N5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" t="s">
         <v>26</v>
       </c>
-      <c r="N5" t="s">
+      <c r="P5" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="A6">
+        <v>10473706</v>
+      </c>
+      <c r="B6">
+        <v>550</v>
+      </c>
+      <c r="C6">
+        <v>0.71</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6">
+        <v>288</v>
+      </c>
+      <c r="J6">
+        <v>416</v>
+      </c>
+      <c r="K6">
+        <v>240</v>
+      </c>
+      <c r="L6" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="M6">
+        <v>96</v>
+      </c>
+      <c r="N6" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="B10">
+        <v>180</v>
+      </c>
+      <c r="C10">
+        <v>0.71</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10">
+        <v>192</v>
+      </c>
+      <c r="J10">
+        <f>129*2</f>
+        <v>258</v>
+      </c>
+      <c r="K10">
+        <v>160</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M10">
+        <v>96</v>
+      </c>
+      <c r="N10" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="B11">
+        <v>180</v>
+      </c>
+      <c r="C11">
+        <v>0.71</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11">
+        <v>193</v>
+      </c>
+      <c r="J11">
+        <f t="shared" ref="J11:J29" si="0">129*2</f>
+        <v>258</v>
+      </c>
+      <c r="K11">
+        <v>160</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M11">
+        <v>96</v>
+      </c>
+      <c r="N11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="B12">
+        <v>180</v>
+      </c>
+      <c r="C12">
+        <v>0.71</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12">
+        <v>194</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K12">
+        <v>160</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M12">
+        <v>96</v>
+      </c>
+      <c r="N12" t="s">
+        <v>28</v>
+      </c>
+      <c r="O12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="B13">
+        <v>180</v>
+      </c>
+      <c r="C13">
+        <v>0.71</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13">
+        <v>195</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K13">
+        <v>160</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M13">
+        <v>96</v>
+      </c>
+      <c r="N13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="B14">
+        <v>180</v>
+      </c>
+      <c r="C14">
+        <v>0.71</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14">
+        <v>6</v>
+      </c>
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14">
+        <v>196</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K14">
+        <v>160</v>
+      </c>
+      <c r="L14" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M14">
+        <v>96</v>
+      </c>
+      <c r="N14" t="s">
+        <v>28</v>
+      </c>
+      <c r="O14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="B15">
+        <v>180</v>
+      </c>
+      <c r="C15">
+        <v>0.71</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15">
+        <v>7</v>
+      </c>
+      <c r="H15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15">
+        <v>197</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K15">
+        <v>160</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M15">
+        <v>96</v>
+      </c>
+      <c r="N15" t="s">
+        <v>28</v>
+      </c>
+      <c r="O15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="B16">
+        <v>180</v>
+      </c>
+      <c r="C16">
+        <v>0.71</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16">
+        <v>8</v>
+      </c>
+      <c r="H16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16">
+        <v>198</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K16">
+        <v>160</v>
+      </c>
+      <c r="L16" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M16">
+        <v>96</v>
+      </c>
+      <c r="N16" t="s">
+        <v>28</v>
+      </c>
+      <c r="O16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="B17">
+        <v>180</v>
+      </c>
+      <c r="C17">
+        <v>0.71</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17">
+        <v>9</v>
+      </c>
+      <c r="H17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17">
+        <v>199</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K17">
+        <v>160</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M17">
+        <v>96</v>
+      </c>
+      <c r="N17" t="s">
+        <v>28</v>
+      </c>
+      <c r="O17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="B18">
+        <v>180</v>
+      </c>
+      <c r="C18">
+        <v>0.71</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18">
+        <v>10</v>
+      </c>
+      <c r="H18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18">
+        <v>200</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K18">
+        <v>160</v>
+      </c>
+      <c r="L18" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M18">
+        <v>96</v>
+      </c>
+      <c r="N18" t="s">
+        <v>28</v>
+      </c>
+      <c r="O18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="B19">
+        <v>180</v>
+      </c>
+      <c r="C19">
+        <v>0.71</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E19" s="2">
+        <v>5</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19">
+        <v>11</v>
+      </c>
+      <c r="H19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19">
+        <v>201</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K19">
+        <v>160</v>
+      </c>
+      <c r="L19" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M19">
+        <v>96</v>
+      </c>
+      <c r="N19" t="s">
+        <v>28</v>
+      </c>
+      <c r="O19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="B20">
+        <v>180</v>
+      </c>
+      <c r="C20">
+        <v>0.71</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20">
+        <v>12</v>
+      </c>
+      <c r="H20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20">
+        <v>202</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K20">
+        <v>160</v>
+      </c>
+      <c r="L20" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M20">
+        <v>96</v>
+      </c>
+      <c r="N20" t="s">
+        <v>28</v>
+      </c>
+      <c r="O20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="B21">
+        <v>180</v>
+      </c>
+      <c r="C21">
+        <v>0.71</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21">
+        <v>13</v>
+      </c>
+      <c r="H21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21">
+        <v>203</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K21">
+        <v>160</v>
+      </c>
+      <c r="L21" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M21">
+        <v>96</v>
+      </c>
+      <c r="N21" t="s">
+        <v>28</v>
+      </c>
+      <c r="O21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="B22">
+        <v>180</v>
+      </c>
+      <c r="C22">
+        <v>0.71</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22">
+        <v>14</v>
+      </c>
+      <c r="H22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22">
+        <v>204</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K22">
+        <v>160</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M22">
+        <v>96</v>
+      </c>
+      <c r="N22" t="s">
+        <v>28</v>
+      </c>
+      <c r="O22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="B23">
+        <v>180</v>
+      </c>
+      <c r="C23">
+        <v>0.71</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E23" s="2">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23">
+        <v>15</v>
+      </c>
+      <c r="H23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23">
+        <v>205</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K23">
+        <v>160</v>
+      </c>
+      <c r="L23" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M23">
+        <v>96</v>
+      </c>
+      <c r="N23" t="s">
+        <v>28</v>
+      </c>
+      <c r="O23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="B24">
+        <v>180</v>
+      </c>
+      <c r="C24">
+        <v>0.71</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E24" s="2">
+        <v>5</v>
+      </c>
+      <c r="F24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24">
+        <v>16</v>
+      </c>
+      <c r="H24" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24">
+        <v>206</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K24">
+        <v>160</v>
+      </c>
+      <c r="L24" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M24">
+        <v>96</v>
+      </c>
+      <c r="N24" t="s">
+        <v>28</v>
+      </c>
+      <c r="O24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="B25">
+        <v>180</v>
+      </c>
+      <c r="C25">
+        <v>0.71</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25">
+        <v>17</v>
+      </c>
+      <c r="H25" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25">
+        <v>207</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K25">
+        <v>160</v>
+      </c>
+      <c r="L25" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M25">
+        <v>96</v>
+      </c>
+      <c r="N25" t="s">
+        <v>28</v>
+      </c>
+      <c r="O25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="B26">
+        <v>180</v>
+      </c>
+      <c r="C26">
+        <v>0.71</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26">
+        <v>18</v>
+      </c>
+      <c r="H26" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26">
+        <v>208</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K26">
+        <v>160</v>
+      </c>
+      <c r="L26" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M26">
+        <v>96</v>
+      </c>
+      <c r="N26" t="s">
+        <v>28</v>
+      </c>
+      <c r="O26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="B27">
+        <v>180</v>
+      </c>
+      <c r="C27">
+        <v>0.71</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27">
+        <v>19</v>
+      </c>
+      <c r="H27" t="s">
+        <v>21</v>
+      </c>
+      <c r="I27">
+        <v>209</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K27">
+        <v>160</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M27">
+        <v>96</v>
+      </c>
+      <c r="N27" t="s">
+        <v>28</v>
+      </c>
+      <c r="O27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="B28">
+        <v>180</v>
+      </c>
+      <c r="C28">
+        <v>0.71</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="E28" s="2">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28">
+        <v>20</v>
+      </c>
+      <c r="H28" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28">
+        <v>210</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K28">
+        <v>160</v>
+      </c>
+      <c r="L28" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M28">
+        <v>96</v>
+      </c>
+      <c r="N28" t="s">
+        <v>28</v>
+      </c>
+      <c r="O28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="B29">
+        <v>180</v>
+      </c>
+      <c r="C29">
+        <v>0.71</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="E29" s="2">
+        <v>5</v>
+      </c>
+      <c r="F29" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29">
+        <v>21</v>
+      </c>
+      <c r="H29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I29">
+        <v>211</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K29">
+        <v>160</v>
+      </c>
+      <c r="L29" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M29">
+        <v>96</v>
+      </c>
+      <c r="N29" t="s">
+        <v>28</v>
+      </c>
+      <c r="O29" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update new case of Re_tau=150
</commit_message>
<xml_diff>
--- a/case_number_20250816.xlsx
+++ b/case_number_20250816.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chang\Nutstore\1\Nutstore\Workspace\convection_time_varying_T\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9A0D1C-681D-476A-B3F2-A0397B27D473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AEFC482-387D-423C-9783-6F238B76BECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="55">
   <si>
     <t>omega</t>
   </si>
@@ -183,15 +183,6 @@
     <t>10 days</t>
   </si>
   <si>
-    <t>2 medmem nodes, each 950GB memory</t>
-  </si>
-  <si>
-    <t>990G</t>
-  </si>
-  <si>
-    <t>killed OOM</t>
-  </si>
-  <si>
     <t>bigmem partition: 1900GB memory</t>
   </si>
   <si>
@@ -208,6 +199,9 @@
   </si>
   <si>
     <t>lambda</t>
+  </si>
+  <si>
+    <t>Validation of Kasagi (1992), continuation of 10424250</t>
   </si>
 </sst>
 </file>
@@ -249,10 +243,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,10 +694,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0792B6-F3DE-44AA-920E-7B8294731BF8}">
-  <dimension ref="A1:R60"/>
+  <dimension ref="A1:Q62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -710,7 +705,7 @@
     <col min="1" max="1" width="31.29296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -763,7 +758,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>10249087</v>
       </c>
@@ -807,7 +802,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -858,7 +853,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>10336395</v>
       </c>
@@ -908,7 +903,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>10337407</v>
       </c>
@@ -955,7 +950,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>10473706</v>
       </c>
@@ -1005,128 +1000,76 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.5">
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.5">
-      <c r="A9">
-        <v>10606860</v>
-      </c>
-      <c r="B9">
-        <v>395</v>
-      </c>
-      <c r="C9">
-        <v>0.71</v>
-      </c>
-      <c r="D9">
+    <row r="9" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="2">
+        <v>10629945</v>
+      </c>
+      <c r="B9" s="2">
+        <v>150</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.71</v>
+      </c>
+      <c r="D9" s="2">
         <v>0</v>
       </c>
-      <c r="F9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9">
+      <c r="F9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="2">
         <v>2</v>
       </c>
-      <c r="H9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9">
-        <v>256</v>
-      </c>
-      <c r="J9">
-        <v>416</v>
-      </c>
-      <c r="K9">
-        <v>240</v>
-      </c>
-      <c r="L9" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="M9">
-        <v>104</v>
-      </c>
-      <c r="N9" t="s">
-        <v>28</v>
-      </c>
-      <c r="O9" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q9" t="s">
+      <c r="H9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="2">
+        <v>192</v>
+      </c>
+      <c r="J9" s="2">
+        <f>129*2</f>
+        <v>258</v>
+      </c>
+      <c r="K9" s="2">
+        <v>160</v>
+      </c>
+      <c r="L9" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="M9" s="2">
+        <v>96</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
         <v>48</v>
       </c>
-      <c r="R9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.5">
-      <c r="A10">
-        <v>10606898</v>
-      </c>
-      <c r="B10">
-        <v>395</v>
-      </c>
-      <c r="C10">
-        <v>0.71</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10">
-        <v>2</v>
-      </c>
-      <c r="H10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10">
-        <v>220</v>
-      </c>
-      <c r="J10">
-        <v>416</v>
-      </c>
-      <c r="K10">
-        <v>210</v>
-      </c>
-      <c r="L10" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="M10">
-        <v>104</v>
-      </c>
-      <c r="N10" t="s">
-        <v>28</v>
-      </c>
-      <c r="O10" t="s">
-        <v>49</v>
-      </c>
-      <c r="P10" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>48</v>
-      </c>
-      <c r="R10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.5">
-      <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.5">
-      <c r="A12" t="s">
-        <v>51</v>
-      </c>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>10611110</v>
       </c>
@@ -1164,21 +1107,21 @@
         <v>104</v>
       </c>
       <c r="N13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="O13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="P13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.5">
       <c r="D16">
         <v>0.1</v>
       </c>
@@ -1203,104 +1146,13 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A20">
-        <v>10525261</v>
-      </c>
       <c r="B20">
-        <v>180</v>
-      </c>
-      <c r="C20">
-        <v>0.71</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20">
-        <v>2</v>
-      </c>
-      <c r="H20" t="s">
-        <v>21</v>
-      </c>
-      <c r="I20">
-        <v>192</v>
-      </c>
-      <c r="J20">
-        <f>129*2</f>
-        <v>258</v>
-      </c>
-      <c r="K20">
-        <v>160</v>
-      </c>
-      <c r="L20" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M20">
-        <v>96</v>
-      </c>
-      <c r="N20" t="s">
-        <v>28</v>
-      </c>
-      <c r="O20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A21">
-        <v>10476429</v>
-      </c>
-      <c r="B21">
-        <v>180</v>
-      </c>
-      <c r="C21">
-        <v>0.71</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F21" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21">
-        <v>2</v>
-      </c>
-      <c r="H21" t="s">
-        <v>21</v>
-      </c>
-      <c r="I21">
-        <v>192</v>
-      </c>
-      <c r="J21">
-        <f>129*2</f>
-        <v>258</v>
-      </c>
-      <c r="K21">
-        <v>160</v>
-      </c>
-      <c r="L21" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M21">
-        <v>96</v>
-      </c>
-      <c r="N21" t="s">
-        <v>28</v>
-      </c>
-      <c r="O21" t="s">
-        <v>46</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A22">
-        <v>10478562</v>
+        <v>10525261</v>
       </c>
       <c r="B22">
         <v>180</v>
@@ -1312,22 +1164,22 @@
         <v>0.1</v>
       </c>
       <c r="E22" s="2">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F22" t="s">
         <v>20</v>
       </c>
       <c r="G22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H22" t="s">
         <v>21</v>
       </c>
       <c r="I22">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J22">
-        <f t="shared" ref="J22:J53" si="0">129*2</f>
+        <f>129*2</f>
         <v>258</v>
       </c>
       <c r="K22">
@@ -1348,7 +1200,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A23">
-        <v>10478905</v>
+        <v>10476429</v>
       </c>
       <c r="B23">
         <v>180</v>
@@ -1360,22 +1212,22 @@
         <v>0.1</v>
       </c>
       <c r="E23" s="2">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F23" t="s">
         <v>20</v>
       </c>
       <c r="G23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H23" t="s">
         <v>21</v>
       </c>
       <c r="I23">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J23">
-        <f t="shared" si="0"/>
+        <f>129*2</f>
         <v>258</v>
       </c>
       <c r="K23">
@@ -1396,7 +1248,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A24">
-        <v>10478910</v>
+        <v>10478562</v>
       </c>
       <c r="B24">
         <v>180</v>
@@ -1408,22 +1260,22 @@
         <v>0.1</v>
       </c>
       <c r="E24" s="2">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F24" t="s">
         <v>20</v>
       </c>
       <c r="G24">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H24" t="s">
         <v>21</v>
       </c>
       <c r="I24">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J24">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J24:J55" si="0">129*2</f>
         <v>258</v>
       </c>
       <c r="K24">
@@ -1444,7 +1296,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A25">
-        <v>10478912</v>
+        <v>10478905</v>
       </c>
       <c r="B25">
         <v>180</v>
@@ -1456,19 +1308,19 @@
         <v>0.1</v>
       </c>
       <c r="E25" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F25" t="s">
         <v>20</v>
       </c>
       <c r="G25">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H25" t="s">
         <v>21</v>
       </c>
       <c r="I25">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J25">
         <f t="shared" si="0"/>
@@ -1491,13 +1343,56 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="L26" s="1"/>
+      <c r="A26">
+        <v>10478910</v>
+      </c>
+      <c r="B26">
+        <v>180</v>
+      </c>
+      <c r="C26">
+        <v>0.71</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26">
+        <v>195</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K26">
+        <v>160</v>
+      </c>
+      <c r="L26" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M26">
+        <v>96</v>
+      </c>
+      <c r="N26" t="s">
+        <v>28</v>
+      </c>
+      <c r="O26" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A27">
-        <v>10526147</v>
+        <v>10478912</v>
       </c>
       <c r="B27">
         <v>180</v>
@@ -1506,22 +1401,22 @@
         <v>0.71</v>
       </c>
       <c r="D27" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E27" s="2">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="F27" t="s">
         <v>20</v>
       </c>
       <c r="G27">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H27" t="s">
         <v>21</v>
       </c>
       <c r="I27">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J27">
         <f t="shared" si="0"/>
@@ -1544,56 +1439,13 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A28">
-        <v>10479023</v>
-      </c>
-      <c r="B28">
-        <v>180</v>
-      </c>
-      <c r="C28">
-        <v>0.71</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="E28" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F28" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28">
-        <v>7</v>
-      </c>
-      <c r="H28" t="s">
-        <v>21</v>
-      </c>
-      <c r="I28">
-        <v>197</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="K28">
-        <v>160</v>
-      </c>
-      <c r="L28" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M28">
-        <v>96</v>
-      </c>
-      <c r="N28" t="s">
-        <v>28</v>
-      </c>
-      <c r="O28" t="s">
-        <v>46</v>
-      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A29">
-        <v>10479256</v>
+        <v>10526147</v>
       </c>
       <c r="B29">
         <v>180</v>
@@ -1605,19 +1457,19 @@
         <v>0.2</v>
       </c>
       <c r="E29" s="2">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F29" t="s">
         <v>20</v>
       </c>
       <c r="G29">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H29" t="s">
         <v>21</v>
       </c>
       <c r="I29">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J29">
         <f t="shared" si="0"/>
@@ -1641,7 +1493,7 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A30">
-        <v>10481244</v>
+        <v>10479023</v>
       </c>
       <c r="B30">
         <v>180</v>
@@ -1653,19 +1505,19 @@
         <v>0.2</v>
       </c>
       <c r="E30" s="2">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F30" t="s">
         <v>20</v>
       </c>
       <c r="G30">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H30" t="s">
         <v>21</v>
       </c>
       <c r="I30">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
@@ -1689,7 +1541,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A31">
-        <v>10481262</v>
+        <v>10479256</v>
       </c>
       <c r="B31">
         <v>180</v>
@@ -1701,19 +1553,19 @@
         <v>0.2</v>
       </c>
       <c r="E31" s="2">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F31" t="s">
         <v>20</v>
       </c>
       <c r="G31">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H31" t="s">
         <v>21</v>
       </c>
       <c r="I31">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
@@ -1737,7 +1589,7 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A32">
-        <v>10481790</v>
+        <v>10481244</v>
       </c>
       <c r="B32">
         <v>180</v>
@@ -1749,19 +1601,19 @@
         <v>0.2</v>
       </c>
       <c r="E32" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F32" t="s">
         <v>20</v>
       </c>
       <c r="G32">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H32" t="s">
         <v>21</v>
       </c>
       <c r="I32">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
@@ -1784,13 +1636,56 @@
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="L33" s="1"/>
+      <c r="A33">
+        <v>10481262</v>
+      </c>
+      <c r="B33">
+        <v>180</v>
+      </c>
+      <c r="C33">
+        <v>0.71</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E33" s="2">
+        <v>2</v>
+      </c>
+      <c r="F33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33">
+        <v>10</v>
+      </c>
+      <c r="H33" t="s">
+        <v>21</v>
+      </c>
+      <c r="I33">
+        <v>200</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K33">
+        <v>160</v>
+      </c>
+      <c r="L33" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M33">
+        <v>96</v>
+      </c>
+      <c r="N33" t="s">
+        <v>28</v>
+      </c>
+      <c r="O33" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A34">
-        <v>10526152</v>
+        <v>10481790</v>
       </c>
       <c r="B34">
         <v>180</v>
@@ -1799,22 +1694,22 @@
         <v>0.71</v>
       </c>
       <c r="D34" s="2">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E34" s="2">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="F34" t="s">
         <v>20</v>
       </c>
       <c r="G34">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H34" t="s">
         <v>21</v>
       </c>
       <c r="I34">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
@@ -1837,56 +1732,13 @@
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A35">
-        <v>10482459</v>
-      </c>
-      <c r="B35">
-        <v>180</v>
-      </c>
-      <c r="C35">
-        <v>0.71</v>
-      </c>
-      <c r="D35" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="E35" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F35" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35">
-        <v>12</v>
-      </c>
-      <c r="H35" t="s">
-        <v>21</v>
-      </c>
-      <c r="I35">
-        <v>202</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="K35">
-        <v>160</v>
-      </c>
-      <c r="L35" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M35">
-        <v>96</v>
-      </c>
-      <c r="N35" t="s">
-        <v>28</v>
-      </c>
-      <c r="O35" t="s">
-        <v>46</v>
-      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="L35" s="1"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A36">
-        <v>10484952</v>
+        <v>10526152</v>
       </c>
       <c r="B36">
         <v>180</v>
@@ -1898,19 +1750,19 @@
         <v>0.3</v>
       </c>
       <c r="E36" s="2">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F36" t="s">
         <v>20</v>
       </c>
       <c r="G36">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H36" t="s">
         <v>21</v>
       </c>
       <c r="I36">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J36">
         <f t="shared" si="0"/>
@@ -1934,7 +1786,7 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A37">
-        <v>10490537</v>
+        <v>10482459</v>
       </c>
       <c r="B37">
         <v>180</v>
@@ -1946,19 +1798,19 @@
         <v>0.3</v>
       </c>
       <c r="E37" s="2">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F37" t="s">
         <v>20</v>
       </c>
       <c r="G37">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H37" t="s">
         <v>21</v>
       </c>
       <c r="I37">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
@@ -1982,7 +1834,7 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A38">
-        <v>10500013</v>
+        <v>10484952</v>
       </c>
       <c r="B38">
         <v>180</v>
@@ -1994,19 +1846,19 @@
         <v>0.3</v>
       </c>
       <c r="E38" s="2">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F38" t="s">
         <v>20</v>
       </c>
       <c r="G38">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H38" t="s">
         <v>21</v>
       </c>
       <c r="I38">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J38">
         <f t="shared" si="0"/>
@@ -2030,7 +1882,7 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A39">
-        <v>10500017</v>
+        <v>10490537</v>
       </c>
       <c r="B39">
         <v>180</v>
@@ -2042,19 +1894,19 @@
         <v>0.3</v>
       </c>
       <c r="E39" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F39" t="s">
         <v>20</v>
       </c>
       <c r="G39">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H39" t="s">
         <v>21</v>
       </c>
       <c r="I39">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
@@ -2077,13 +1929,56 @@
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="L40" s="1"/>
+      <c r="A40">
+        <v>10500013</v>
+      </c>
+      <c r="B40">
+        <v>180</v>
+      </c>
+      <c r="C40">
+        <v>0.71</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E40" s="2">
+        <v>2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G40">
+        <v>15</v>
+      </c>
+      <c r="H40" t="s">
+        <v>21</v>
+      </c>
+      <c r="I40">
+        <v>205</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K40">
+        <v>160</v>
+      </c>
+      <c r="L40" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M40">
+        <v>96</v>
+      </c>
+      <c r="N40" t="s">
+        <v>28</v>
+      </c>
+      <c r="O40" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A41">
-        <v>10526156</v>
+        <v>10500017</v>
       </c>
       <c r="B41">
         <v>180</v>
@@ -2092,22 +1987,22 @@
         <v>0.71</v>
       </c>
       <c r="D41" s="2">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="E41" s="2">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="F41" t="s">
         <v>20</v>
       </c>
       <c r="G41">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H41" t="s">
         <v>21</v>
       </c>
       <c r="I41">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
@@ -2130,56 +2025,13 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A42">
-        <v>10500654</v>
-      </c>
-      <c r="B42">
-        <v>180</v>
-      </c>
-      <c r="C42">
-        <v>0.71</v>
-      </c>
-      <c r="D42" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="E42" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F42" t="s">
-        <v>20</v>
-      </c>
-      <c r="G42">
-        <v>17</v>
-      </c>
-      <c r="H42" t="s">
-        <v>21</v>
-      </c>
-      <c r="I42">
-        <v>207</v>
-      </c>
-      <c r="J42">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="K42">
-        <v>160</v>
-      </c>
-      <c r="L42" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M42">
-        <v>96</v>
-      </c>
-      <c r="N42" t="s">
-        <v>28</v>
-      </c>
-      <c r="O42" t="s">
-        <v>46</v>
-      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="L42" s="1"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A43">
-        <v>10501196</v>
+        <v>10526156</v>
       </c>
       <c r="B43">
         <v>180</v>
@@ -2191,19 +2043,19 @@
         <v>0.4</v>
       </c>
       <c r="E43" s="2">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F43" t="s">
         <v>20</v>
       </c>
       <c r="G43">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H43" t="s">
         <v>21</v>
       </c>
       <c r="I43">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
@@ -2227,7 +2079,7 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A44">
-        <v>10501212</v>
+        <v>10500654</v>
       </c>
       <c r="B44">
         <v>180</v>
@@ -2239,19 +2091,19 @@
         <v>0.4</v>
       </c>
       <c r="E44" s="2">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F44" t="s">
         <v>20</v>
       </c>
       <c r="G44">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H44" t="s">
         <v>21</v>
       </c>
       <c r="I44">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
@@ -2275,7 +2127,7 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A45">
-        <v>10501276</v>
+        <v>10501196</v>
       </c>
       <c r="B45">
         <v>180</v>
@@ -2287,19 +2139,19 @@
         <v>0.4</v>
       </c>
       <c r="E45" s="2">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F45" t="s">
         <v>20</v>
       </c>
       <c r="G45">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H45" t="s">
         <v>21</v>
       </c>
       <c r="I45">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
@@ -2323,7 +2175,7 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A46">
-        <v>10507648</v>
+        <v>10501212</v>
       </c>
       <c r="B46">
         <v>180</v>
@@ -2335,19 +2187,19 @@
         <v>0.4</v>
       </c>
       <c r="E46" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F46" t="s">
         <v>20</v>
       </c>
       <c r="G46">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H46" t="s">
         <v>21</v>
       </c>
       <c r="I46">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
@@ -2370,13 +2222,56 @@
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="L47" s="1"/>
+      <c r="A47">
+        <v>10501276</v>
+      </c>
+      <c r="B47">
+        <v>180</v>
+      </c>
+      <c r="C47">
+        <v>0.71</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="E47" s="2">
+        <v>2</v>
+      </c>
+      <c r="F47" t="s">
+        <v>20</v>
+      </c>
+      <c r="G47">
+        <v>20</v>
+      </c>
+      <c r="H47" t="s">
+        <v>21</v>
+      </c>
+      <c r="I47">
+        <v>210</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K47">
+        <v>160</v>
+      </c>
+      <c r="L47" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M47">
+        <v>96</v>
+      </c>
+      <c r="N47" t="s">
+        <v>28</v>
+      </c>
+      <c r="O47" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A48">
-        <v>10526159</v>
+        <v>10507648</v>
       </c>
       <c r="B48">
         <v>180</v>
@@ -2385,22 +2280,22 @@
         <v>0.71</v>
       </c>
       <c r="D48" s="2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E48" s="2">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="F48" t="s">
         <v>20</v>
       </c>
       <c r="G48">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H48" t="s">
         <v>21</v>
       </c>
       <c r="I48">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
@@ -2423,56 +2318,13 @@
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A49">
-        <v>10512815</v>
-      </c>
-      <c r="B49">
-        <v>180</v>
-      </c>
-      <c r="C49">
-        <v>0.71</v>
-      </c>
-      <c r="D49" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E49" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F49" t="s">
-        <v>20</v>
-      </c>
-      <c r="G49">
-        <v>17</v>
-      </c>
-      <c r="H49" t="s">
-        <v>21</v>
-      </c>
-      <c r="I49">
-        <v>207</v>
-      </c>
-      <c r="J49">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="K49">
-        <v>160</v>
-      </c>
-      <c r="L49" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M49">
-        <v>96</v>
-      </c>
-      <c r="N49" t="s">
-        <v>28</v>
-      </c>
-      <c r="O49" t="s">
-        <v>46</v>
-      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="L49" s="1"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A50">
-        <v>10512816</v>
+        <v>10526159</v>
       </c>
       <c r="B50">
         <v>180</v>
@@ -2484,19 +2336,19 @@
         <v>0.5</v>
       </c>
       <c r="E50" s="2">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F50" t="s">
         <v>20</v>
       </c>
       <c r="G50">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H50" t="s">
         <v>21</v>
       </c>
       <c r="I50">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
@@ -2520,7 +2372,7 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A51">
-        <v>10512818</v>
+        <v>10512815</v>
       </c>
       <c r="B51">
         <v>180</v>
@@ -2532,19 +2384,19 @@
         <v>0.5</v>
       </c>
       <c r="E51" s="2">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F51" t="s">
         <v>20</v>
       </c>
       <c r="G51">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H51" t="s">
         <v>21</v>
       </c>
       <c r="I51">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
@@ -2568,7 +2420,7 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A52">
-        <v>10513758</v>
+        <v>10512816</v>
       </c>
       <c r="B52">
         <v>180</v>
@@ -2580,19 +2432,19 @@
         <v>0.5</v>
       </c>
       <c r="E52" s="2">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F52" t="s">
         <v>20</v>
       </c>
       <c r="G52">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H52" t="s">
         <v>21</v>
       </c>
       <c r="I52">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
@@ -2616,7 +2468,7 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A53">
-        <v>10514336</v>
+        <v>10512818</v>
       </c>
       <c r="B53">
         <v>180</v>
@@ -2628,19 +2480,19 @@
         <v>0.5</v>
       </c>
       <c r="E53" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F53" t="s">
         <v>20</v>
       </c>
       <c r="G53">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H53" t="s">
         <v>21</v>
       </c>
       <c r="I53">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
@@ -2662,154 +2514,154 @@
         <v>46</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A56" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="B57" t="s">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A54">
+        <v>10513758</v>
+      </c>
+      <c r="B54">
+        <v>180</v>
+      </c>
+      <c r="C54">
+        <v>0.71</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E54" s="2">
+        <v>2</v>
+      </c>
+      <c r="F54" t="s">
+        <v>20</v>
+      </c>
+      <c r="G54">
+        <v>20</v>
+      </c>
+      <c r="H54" t="s">
+        <v>21</v>
+      </c>
+      <c r="I54">
+        <v>210</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K54">
+        <v>160</v>
+      </c>
+      <c r="L54" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M54">
+        <v>96</v>
+      </c>
+      <c r="N54" t="s">
+        <v>28</v>
+      </c>
+      <c r="O54" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A55">
+        <v>10514336</v>
+      </c>
+      <c r="B55">
+        <v>180</v>
+      </c>
+      <c r="C55">
+        <v>0.71</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E55" s="2">
+        <v>5</v>
+      </c>
+      <c r="F55" t="s">
+        <v>20</v>
+      </c>
+      <c r="G55">
+        <v>21</v>
+      </c>
+      <c r="H55" t="s">
+        <v>21</v>
+      </c>
+      <c r="I55">
+        <v>211</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K55">
+        <v>160</v>
+      </c>
+      <c r="L55" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M55">
+        <v>96</v>
+      </c>
+      <c r="N55" t="s">
+        <v>28</v>
+      </c>
+      <c r="O55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A58" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="B59" t="s">
         <v>16</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C59" t="s">
         <v>4</v>
       </c>
-      <c r="D57" t="s">
-        <v>55</v>
-      </c>
-      <c r="E57" t="s">
-        <v>56</v>
-      </c>
-      <c r="F57" t="s">
+      <c r="D59" t="s">
+        <v>52</v>
+      </c>
+      <c r="E59" t="s">
+        <v>53</v>
+      </c>
+      <c r="F59" t="s">
         <v>5</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G59" t="s">
         <v>7</v>
       </c>
-      <c r="H57" t="s">
+      <c r="H59" t="s">
         <v>8</v>
       </c>
-      <c r="I57" t="s">
+      <c r="I59" t="s">
         <v>17</v>
       </c>
-      <c r="J57" t="s">
+      <c r="J59" t="s">
         <v>18</v>
       </c>
-      <c r="K57" t="s">
+      <c r="K59" t="s">
         <v>19</v>
       </c>
-      <c r="L57" t="s">
+      <c r="L59" t="s">
         <v>29</v>
       </c>
-      <c r="M57" t="s">
+      <c r="M59" t="s">
         <v>27</v>
       </c>
-      <c r="N57" t="s">
+      <c r="N59" t="s">
         <v>23</v>
       </c>
-      <c r="O57" t="s">
+      <c r="O59" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A58">
-        <v>10617236</v>
-      </c>
-      <c r="B58">
-        <v>180</v>
-      </c>
-      <c r="C58">
-        <v>0.71</v>
-      </c>
-      <c r="D58" s="2">
-        <v>120</v>
-      </c>
-      <c r="E58" s="2">
-        <v>0</v>
-      </c>
-      <c r="F58" t="s">
-        <v>20</v>
-      </c>
-      <c r="G58">
-        <v>2</v>
-      </c>
-      <c r="H58" t="s">
-        <v>21</v>
-      </c>
-      <c r="I58">
-        <v>192</v>
-      </c>
-      <c r="J58">
-        <f>129*2</f>
-        <v>258</v>
-      </c>
-      <c r="K58">
-        <v>160</v>
-      </c>
-      <c r="L58" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M58">
-        <v>96</v>
-      </c>
-      <c r="N58" t="s">
-        <v>28</v>
-      </c>
-      <c r="O58" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A59">
-        <v>10622304</v>
-      </c>
-      <c r="B59">
-        <v>180</v>
-      </c>
-      <c r="C59">
-        <v>0.71</v>
-      </c>
-      <c r="D59" s="2">
-        <v>480</v>
-      </c>
-      <c r="E59" s="2">
-        <v>0</v>
-      </c>
-      <c r="F59" t="s">
-        <v>20</v>
-      </c>
-      <c r="G59">
-        <v>2</v>
-      </c>
-      <c r="H59" t="s">
-        <v>21</v>
-      </c>
-      <c r="I59">
-        <v>192</v>
-      </c>
-      <c r="J59">
-        <f>129*2</f>
-        <v>258</v>
-      </c>
-      <c r="K59">
-        <v>160</v>
-      </c>
-      <c r="L59" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M59">
-        <v>96</v>
-      </c>
-      <c r="N59" t="s">
-        <v>28</v>
-      </c>
-      <c r="O59" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A60">
-        <v>10622305</v>
+        <v>10617236</v>
       </c>
       <c r="B60">
         <v>180</v>
@@ -2818,7 +2670,7 @@
         <v>0.71</v>
       </c>
       <c r="D60" s="2">
-        <v>960</v>
+        <v>120</v>
       </c>
       <c r="E60" s="2">
         <v>0</v>
@@ -2852,6 +2704,102 @@
         <v>28</v>
       </c>
       <c r="O60" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A61">
+        <v>10622304</v>
+      </c>
+      <c r="B61">
+        <v>180</v>
+      </c>
+      <c r="C61">
+        <v>0.71</v>
+      </c>
+      <c r="D61" s="2">
+        <v>480</v>
+      </c>
+      <c r="E61" s="2">
+        <v>0</v>
+      </c>
+      <c r="F61" t="s">
+        <v>20</v>
+      </c>
+      <c r="G61">
+        <v>2</v>
+      </c>
+      <c r="H61" t="s">
+        <v>21</v>
+      </c>
+      <c r="I61">
+        <v>192</v>
+      </c>
+      <c r="J61">
+        <f>129*2</f>
+        <v>258</v>
+      </c>
+      <c r="K61">
+        <v>160</v>
+      </c>
+      <c r="L61" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M61">
+        <v>96</v>
+      </c>
+      <c r="N61" t="s">
+        <v>28</v>
+      </c>
+      <c r="O61" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A62">
+        <v>10622305</v>
+      </c>
+      <c r="B62">
+        <v>180</v>
+      </c>
+      <c r="C62">
+        <v>0.71</v>
+      </c>
+      <c r="D62" s="2">
+        <v>960</v>
+      </c>
+      <c r="E62" s="2">
+        <v>0</v>
+      </c>
+      <c r="F62" t="s">
+        <v>20</v>
+      </c>
+      <c r="G62">
+        <v>2</v>
+      </c>
+      <c r="H62" t="s">
+        <v>21</v>
+      </c>
+      <c r="I62">
+        <v>192</v>
+      </c>
+      <c r="J62">
+        <f>129*2</f>
+        <v>258</v>
+      </c>
+      <c r="K62">
+        <v>160</v>
+      </c>
+      <c r="L62" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M62">
+        <v>96</v>
+      </c>
+      <c r="N62" t="s">
+        <v>28</v>
+      </c>
+      <c r="O62" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update the stably stratified version
</commit_message>
<xml_diff>
--- a/case_number_20250816.xlsx
+++ b/case_number_20250816.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chang\Nutstore\1\Nutstore\Workspace\convection_time_varying_T\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AEFC482-387D-423C-9783-6F238B76BECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0F3E3A-F381-412F-825F-1611D1715BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="57">
   <si>
     <t>omega</t>
   </si>
@@ -202,6 +202,12 @@
   </si>
   <si>
     <t>Validation of Kasagi (1992), continuation of 10424250</t>
+  </si>
+  <si>
+    <t>2 days</t>
+  </si>
+  <si>
+    <t>continue at t=4 from 10611110</t>
   </si>
 </sst>
 </file>
@@ -694,10 +700,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0792B6-F3DE-44AA-920E-7B8294731BF8}">
-  <dimension ref="A1:Q62"/>
+  <dimension ref="A1:Q64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1113,28 +1119,65 @@
         <v>49</v>
       </c>
       <c r="P13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="A14">
+        <v>10642100</v>
+      </c>
+      <c r="B14">
+        <v>395</v>
+      </c>
+      <c r="C14">
+        <v>0.71</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14">
+        <v>256</v>
+      </c>
+      <c r="J14">
+        <v>416</v>
+      </c>
+      <c r="K14">
+        <v>240</v>
+      </c>
+      <c r="L14" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="M14">
+        <v>104</v>
+      </c>
+      <c r="N14" t="s">
+        <v>50</v>
+      </c>
+      <c r="O14" t="s">
+        <v>49</v>
+      </c>
+      <c r="P14" t="s">
         <v>47</v>
       </c>
+      <c r="Q14" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="A15" t="s">
+      <c r="L15" s="1"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="D16">
-        <v>0.1</v>
-      </c>
-      <c r="E16">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="D17">
-        <v>0.1</v>
-      </c>
-      <c r="E17">
-        <v>0.05</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.5">
@@ -1142,113 +1185,33 @@
         <v>0.1</v>
       </c>
       <c r="E18">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="D19">
         <v>0.1</v>
       </c>
+      <c r="E19">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="B20">
+      <c r="D20">
+        <v>0.1</v>
+      </c>
+      <c r="E20">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="B22">
         <v>150</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A22">
-        <v>10525261</v>
-      </c>
-      <c r="B22">
-        <v>180</v>
-      </c>
-      <c r="C22">
-        <v>0.71</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F22" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22">
-        <v>2</v>
-      </c>
-      <c r="H22" t="s">
-        <v>21</v>
-      </c>
-      <c r="I22">
-        <v>192</v>
-      </c>
-      <c r="J22">
-        <f>129*2</f>
-        <v>258</v>
-      </c>
-      <c r="K22">
-        <v>160</v>
-      </c>
-      <c r="L22" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M22">
-        <v>96</v>
-      </c>
-      <c r="N22" t="s">
-        <v>28</v>
-      </c>
-      <c r="O22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A23">
-        <v>10476429</v>
-      </c>
-      <c r="B23">
-        <v>180</v>
-      </c>
-      <c r="C23">
-        <v>0.71</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F23" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23">
-        <v>2</v>
-      </c>
-      <c r="H23" t="s">
-        <v>21</v>
-      </c>
-      <c r="I23">
-        <v>192</v>
-      </c>
-      <c r="J23">
-        <f>129*2</f>
-        <v>258</v>
-      </c>
-      <c r="K23">
-        <v>160</v>
-      </c>
-      <c r="L23" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M23">
-        <v>96</v>
-      </c>
-      <c r="N23" t="s">
-        <v>28</v>
-      </c>
-      <c r="O23" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A24">
-        <v>10478562</v>
+        <v>10525261</v>
       </c>
       <c r="B24">
         <v>180</v>
@@ -1260,22 +1223,22 @@
         <v>0.1</v>
       </c>
       <c r="E24" s="2">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F24" t="s">
         <v>20</v>
       </c>
       <c r="G24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H24" t="s">
         <v>21</v>
       </c>
       <c r="I24">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J24">
-        <f t="shared" ref="J24:J55" si="0">129*2</f>
+        <f>129*2</f>
         <v>258</v>
       </c>
       <c r="K24">
@@ -1296,7 +1259,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A25">
-        <v>10478905</v>
+        <v>10476429</v>
       </c>
       <c r="B25">
         <v>180</v>
@@ -1308,22 +1271,22 @@
         <v>0.1</v>
       </c>
       <c r="E25" s="2">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F25" t="s">
         <v>20</v>
       </c>
       <c r="G25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H25" t="s">
         <v>21</v>
       </c>
       <c r="I25">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J25">
-        <f t="shared" si="0"/>
+        <f>129*2</f>
         <v>258</v>
       </c>
       <c r="K25">
@@ -1344,7 +1307,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A26">
-        <v>10478910</v>
+        <v>10478562</v>
       </c>
       <c r="B26">
         <v>180</v>
@@ -1356,22 +1319,22 @@
         <v>0.1</v>
       </c>
       <c r="E26" s="2">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F26" t="s">
         <v>20</v>
       </c>
       <c r="G26">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H26" t="s">
         <v>21</v>
       </c>
       <c r="I26">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J26">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J26:J57" si="0">129*2</f>
         <v>258</v>
       </c>
       <c r="K26">
@@ -1392,7 +1355,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A27">
-        <v>10478912</v>
+        <v>10478905</v>
       </c>
       <c r="B27">
         <v>180</v>
@@ -1404,19 +1367,19 @@
         <v>0.1</v>
       </c>
       <c r="E27" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F27" t="s">
         <v>20</v>
       </c>
       <c r="G27">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H27" t="s">
         <v>21</v>
       </c>
       <c r="I27">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J27">
         <f t="shared" si="0"/>
@@ -1439,13 +1402,56 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="L28" s="1"/>
+      <c r="A28">
+        <v>10478910</v>
+      </c>
+      <c r="B28">
+        <v>180</v>
+      </c>
+      <c r="C28">
+        <v>0.71</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E28" s="2">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28">
+        <v>5</v>
+      </c>
+      <c r="H28" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28">
+        <v>195</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K28">
+        <v>160</v>
+      </c>
+      <c r="L28" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M28">
+        <v>96</v>
+      </c>
+      <c r="N28" t="s">
+        <v>28</v>
+      </c>
+      <c r="O28" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A29">
-        <v>10526147</v>
+        <v>10478912</v>
       </c>
       <c r="B29">
         <v>180</v>
@@ -1454,22 +1460,22 @@
         <v>0.71</v>
       </c>
       <c r="D29" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E29" s="2">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="F29" t="s">
         <v>20</v>
       </c>
       <c r="G29">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H29" t="s">
         <v>21</v>
       </c>
       <c r="I29">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J29">
         <f t="shared" si="0"/>
@@ -1492,56 +1498,13 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A30">
-        <v>10479023</v>
-      </c>
-      <c r="B30">
-        <v>180</v>
-      </c>
-      <c r="C30">
-        <v>0.71</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="E30" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30">
-        <v>7</v>
-      </c>
-      <c r="H30" t="s">
-        <v>21</v>
-      </c>
-      <c r="I30">
-        <v>197</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="K30">
-        <v>160</v>
-      </c>
-      <c r="L30" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M30">
-        <v>96</v>
-      </c>
-      <c r="N30" t="s">
-        <v>28</v>
-      </c>
-      <c r="O30" t="s">
-        <v>46</v>
-      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A31">
-        <v>10479256</v>
+        <v>10526147</v>
       </c>
       <c r="B31">
         <v>180</v>
@@ -1553,19 +1516,19 @@
         <v>0.2</v>
       </c>
       <c r="E31" s="2">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F31" t="s">
         <v>20</v>
       </c>
       <c r="G31">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H31" t="s">
         <v>21</v>
       </c>
       <c r="I31">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
@@ -1589,7 +1552,7 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A32">
-        <v>10481244</v>
+        <v>10479023</v>
       </c>
       <c r="B32">
         <v>180</v>
@@ -1601,19 +1564,19 @@
         <v>0.2</v>
       </c>
       <c r="E32" s="2">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F32" t="s">
         <v>20</v>
       </c>
       <c r="G32">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H32" t="s">
         <v>21</v>
       </c>
       <c r="I32">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
@@ -1637,7 +1600,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A33">
-        <v>10481262</v>
+        <v>10479256</v>
       </c>
       <c r="B33">
         <v>180</v>
@@ -1649,19 +1612,19 @@
         <v>0.2</v>
       </c>
       <c r="E33" s="2">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F33" t="s">
         <v>20</v>
       </c>
       <c r="G33">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H33" t="s">
         <v>21</v>
       </c>
       <c r="I33">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
@@ -1685,7 +1648,7 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A34">
-        <v>10481790</v>
+        <v>10481244</v>
       </c>
       <c r="B34">
         <v>180</v>
@@ -1697,19 +1660,19 @@
         <v>0.2</v>
       </c>
       <c r="E34" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F34" t="s">
         <v>20</v>
       </c>
       <c r="G34">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H34" t="s">
         <v>21</v>
       </c>
       <c r="I34">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
@@ -1732,13 +1695,56 @@
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="L35" s="1"/>
+      <c r="A35">
+        <v>10481262</v>
+      </c>
+      <c r="B35">
+        <v>180</v>
+      </c>
+      <c r="C35">
+        <v>0.71</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E35" s="2">
+        <v>2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35">
+        <v>10</v>
+      </c>
+      <c r="H35" t="s">
+        <v>21</v>
+      </c>
+      <c r="I35">
+        <v>200</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K35">
+        <v>160</v>
+      </c>
+      <c r="L35" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M35">
+        <v>96</v>
+      </c>
+      <c r="N35" t="s">
+        <v>28</v>
+      </c>
+      <c r="O35" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A36">
-        <v>10526152</v>
+        <v>10481790</v>
       </c>
       <c r="B36">
         <v>180</v>
@@ -1747,22 +1753,22 @@
         <v>0.71</v>
       </c>
       <c r="D36" s="2">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E36" s="2">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="F36" t="s">
         <v>20</v>
       </c>
       <c r="G36">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H36" t="s">
         <v>21</v>
       </c>
       <c r="I36">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J36">
         <f t="shared" si="0"/>
@@ -1785,56 +1791,13 @@
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A37">
-        <v>10482459</v>
-      </c>
-      <c r="B37">
-        <v>180</v>
-      </c>
-      <c r="C37">
-        <v>0.71</v>
-      </c>
-      <c r="D37" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="E37" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F37" t="s">
-        <v>20</v>
-      </c>
-      <c r="G37">
-        <v>12</v>
-      </c>
-      <c r="H37" t="s">
-        <v>21</v>
-      </c>
-      <c r="I37">
-        <v>202</v>
-      </c>
-      <c r="J37">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="K37">
-        <v>160</v>
-      </c>
-      <c r="L37" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M37">
-        <v>96</v>
-      </c>
-      <c r="N37" t="s">
-        <v>28</v>
-      </c>
-      <c r="O37" t="s">
-        <v>46</v>
-      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="L37" s="1"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A38">
-        <v>10484952</v>
+        <v>10526152</v>
       </c>
       <c r="B38">
         <v>180</v>
@@ -1846,19 +1809,19 @@
         <v>0.3</v>
       </c>
       <c r="E38" s="2">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F38" t="s">
         <v>20</v>
       </c>
       <c r="G38">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H38" t="s">
         <v>21</v>
       </c>
       <c r="I38">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J38">
         <f t="shared" si="0"/>
@@ -1882,7 +1845,7 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A39">
-        <v>10490537</v>
+        <v>10482459</v>
       </c>
       <c r="B39">
         <v>180</v>
@@ -1894,19 +1857,19 @@
         <v>0.3</v>
       </c>
       <c r="E39" s="2">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F39" t="s">
         <v>20</v>
       </c>
       <c r="G39">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H39" t="s">
         <v>21</v>
       </c>
       <c r="I39">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
@@ -1930,7 +1893,7 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A40">
-        <v>10500013</v>
+        <v>10484952</v>
       </c>
       <c r="B40">
         <v>180</v>
@@ -1942,19 +1905,19 @@
         <v>0.3</v>
       </c>
       <c r="E40" s="2">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F40" t="s">
         <v>20</v>
       </c>
       <c r="G40">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H40" t="s">
         <v>21</v>
       </c>
       <c r="I40">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
@@ -1978,7 +1941,7 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A41">
-        <v>10500017</v>
+        <v>10490537</v>
       </c>
       <c r="B41">
         <v>180</v>
@@ -1990,19 +1953,19 @@
         <v>0.3</v>
       </c>
       <c r="E41" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F41" t="s">
         <v>20</v>
       </c>
       <c r="G41">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H41" t="s">
         <v>21</v>
       </c>
       <c r="I41">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
@@ -2025,13 +1988,56 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="L42" s="1"/>
+      <c r="A42">
+        <v>10500013</v>
+      </c>
+      <c r="B42">
+        <v>180</v>
+      </c>
+      <c r="C42">
+        <v>0.71</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E42" s="2">
+        <v>2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>20</v>
+      </c>
+      <c r="G42">
+        <v>15</v>
+      </c>
+      <c r="H42" t="s">
+        <v>21</v>
+      </c>
+      <c r="I42">
+        <v>205</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K42">
+        <v>160</v>
+      </c>
+      <c r="L42" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M42">
+        <v>96</v>
+      </c>
+      <c r="N42" t="s">
+        <v>28</v>
+      </c>
+      <c r="O42" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A43">
-        <v>10526156</v>
+        <v>10500017</v>
       </c>
       <c r="B43">
         <v>180</v>
@@ -2040,22 +2046,22 @@
         <v>0.71</v>
       </c>
       <c r="D43" s="2">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="E43" s="2">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="F43" t="s">
         <v>20</v>
       </c>
       <c r="G43">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H43" t="s">
         <v>21</v>
       </c>
       <c r="I43">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
@@ -2078,56 +2084,13 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A44">
-        <v>10500654</v>
-      </c>
-      <c r="B44">
-        <v>180</v>
-      </c>
-      <c r="C44">
-        <v>0.71</v>
-      </c>
-      <c r="D44" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="E44" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F44" t="s">
-        <v>20</v>
-      </c>
-      <c r="G44">
-        <v>17</v>
-      </c>
-      <c r="H44" t="s">
-        <v>21</v>
-      </c>
-      <c r="I44">
-        <v>207</v>
-      </c>
-      <c r="J44">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="K44">
-        <v>160</v>
-      </c>
-      <c r="L44" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M44">
-        <v>96</v>
-      </c>
-      <c r="N44" t="s">
-        <v>28</v>
-      </c>
-      <c r="O44" t="s">
-        <v>46</v>
-      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="L44" s="1"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A45">
-        <v>10501196</v>
+        <v>10526156</v>
       </c>
       <c r="B45">
         <v>180</v>
@@ -2139,19 +2102,19 @@
         <v>0.4</v>
       </c>
       <c r="E45" s="2">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F45" t="s">
         <v>20</v>
       </c>
       <c r="G45">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H45" t="s">
         <v>21</v>
       </c>
       <c r="I45">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
@@ -2175,7 +2138,7 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A46">
-        <v>10501212</v>
+        <v>10500654</v>
       </c>
       <c r="B46">
         <v>180</v>
@@ -2187,19 +2150,19 @@
         <v>0.4</v>
       </c>
       <c r="E46" s="2">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F46" t="s">
         <v>20</v>
       </c>
       <c r="G46">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H46" t="s">
         <v>21</v>
       </c>
       <c r="I46">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
@@ -2223,7 +2186,7 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A47">
-        <v>10501276</v>
+        <v>10501196</v>
       </c>
       <c r="B47">
         <v>180</v>
@@ -2235,19 +2198,19 @@
         <v>0.4</v>
       </c>
       <c r="E47" s="2">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F47" t="s">
         <v>20</v>
       </c>
       <c r="G47">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H47" t="s">
         <v>21</v>
       </c>
       <c r="I47">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
@@ -2271,7 +2234,7 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A48">
-        <v>10507648</v>
+        <v>10501212</v>
       </c>
       <c r="B48">
         <v>180</v>
@@ -2283,19 +2246,19 @@
         <v>0.4</v>
       </c>
       <c r="E48" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F48" t="s">
         <v>20</v>
       </c>
       <c r="G48">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H48" t="s">
         <v>21</v>
       </c>
       <c r="I48">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
@@ -2318,13 +2281,56 @@
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="L49" s="1"/>
+      <c r="A49">
+        <v>10501276</v>
+      </c>
+      <c r="B49">
+        <v>180</v>
+      </c>
+      <c r="C49">
+        <v>0.71</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="E49" s="2">
+        <v>2</v>
+      </c>
+      <c r="F49" t="s">
+        <v>20</v>
+      </c>
+      <c r="G49">
+        <v>20</v>
+      </c>
+      <c r="H49" t="s">
+        <v>21</v>
+      </c>
+      <c r="I49">
+        <v>210</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K49">
+        <v>160</v>
+      </c>
+      <c r="L49" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M49">
+        <v>96</v>
+      </c>
+      <c r="N49" t="s">
+        <v>28</v>
+      </c>
+      <c r="O49" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A50">
-        <v>10526159</v>
+        <v>10507648</v>
       </c>
       <c r="B50">
         <v>180</v>
@@ -2333,22 +2339,22 @@
         <v>0.71</v>
       </c>
       <c r="D50" s="2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E50" s="2">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="F50" t="s">
         <v>20</v>
       </c>
       <c r="G50">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H50" t="s">
         <v>21</v>
       </c>
       <c r="I50">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
@@ -2371,56 +2377,13 @@
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A51">
-        <v>10512815</v>
-      </c>
-      <c r="B51">
-        <v>180</v>
-      </c>
-      <c r="C51">
-        <v>0.71</v>
-      </c>
-      <c r="D51" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E51" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F51" t="s">
-        <v>20</v>
-      </c>
-      <c r="G51">
-        <v>17</v>
-      </c>
-      <c r="H51" t="s">
-        <v>21</v>
-      </c>
-      <c r="I51">
-        <v>207</v>
-      </c>
-      <c r="J51">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="K51">
-        <v>160</v>
-      </c>
-      <c r="L51" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M51">
-        <v>96</v>
-      </c>
-      <c r="N51" t="s">
-        <v>28</v>
-      </c>
-      <c r="O51" t="s">
-        <v>46</v>
-      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="L51" s="1"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A52">
-        <v>10512816</v>
+        <v>10526159</v>
       </c>
       <c r="B52">
         <v>180</v>
@@ -2432,19 +2395,19 @@
         <v>0.5</v>
       </c>
       <c r="E52" s="2">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F52" t="s">
         <v>20</v>
       </c>
       <c r="G52">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H52" t="s">
         <v>21</v>
       </c>
       <c r="I52">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
@@ -2468,7 +2431,7 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A53">
-        <v>10512818</v>
+        <v>10512815</v>
       </c>
       <c r="B53">
         <v>180</v>
@@ -2480,19 +2443,19 @@
         <v>0.5</v>
       </c>
       <c r="E53" s="2">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F53" t="s">
         <v>20</v>
       </c>
       <c r="G53">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H53" t="s">
         <v>21</v>
       </c>
       <c r="I53">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
@@ -2516,7 +2479,7 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A54">
-        <v>10513758</v>
+        <v>10512816</v>
       </c>
       <c r="B54">
         <v>180</v>
@@ -2528,19 +2491,19 @@
         <v>0.5</v>
       </c>
       <c r="E54" s="2">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F54" t="s">
         <v>20</v>
       </c>
       <c r="G54">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H54" t="s">
         <v>21</v>
       </c>
       <c r="I54">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
@@ -2564,7 +2527,7 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A55">
-        <v>10514336</v>
+        <v>10512818</v>
       </c>
       <c r="B55">
         <v>180</v>
@@ -2576,19 +2539,19 @@
         <v>0.5</v>
       </c>
       <c r="E55" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F55" t="s">
         <v>20</v>
       </c>
       <c r="G55">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H55" t="s">
         <v>21</v>
       </c>
       <c r="I55">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J55">
         <f t="shared" si="0"/>
@@ -2610,154 +2573,154 @@
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A58" t="s">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A56">
+        <v>10513758</v>
+      </c>
+      <c r="B56">
+        <v>180</v>
+      </c>
+      <c r="C56">
+        <v>0.71</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E56" s="2">
+        <v>2</v>
+      </c>
+      <c r="F56" t="s">
+        <v>20</v>
+      </c>
+      <c r="G56">
+        <v>20</v>
+      </c>
+      <c r="H56" t="s">
+        <v>21</v>
+      </c>
+      <c r="I56">
+        <v>210</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K56">
+        <v>160</v>
+      </c>
+      <c r="L56" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M56">
+        <v>96</v>
+      </c>
+      <c r="N56" t="s">
+        <v>28</v>
+      </c>
+      <c r="O56" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A57">
+        <v>10514336</v>
+      </c>
+      <c r="B57">
+        <v>180</v>
+      </c>
+      <c r="C57">
+        <v>0.71</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E57" s="2">
+        <v>5</v>
+      </c>
+      <c r="F57" t="s">
+        <v>20</v>
+      </c>
+      <c r="G57">
+        <v>21</v>
+      </c>
+      <c r="H57" t="s">
+        <v>21</v>
+      </c>
+      <c r="I57">
+        <v>211</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K57">
+        <v>160</v>
+      </c>
+      <c r="L57" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M57">
+        <v>96</v>
+      </c>
+      <c r="N57" t="s">
+        <v>28</v>
+      </c>
+      <c r="O57" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A60" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="B59" t="s">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="B61" t="s">
         <v>16</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C61" t="s">
         <v>4</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D61" t="s">
         <v>52</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E61" t="s">
         <v>53</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F61" t="s">
         <v>5</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G61" t="s">
         <v>7</v>
       </c>
-      <c r="H59" t="s">
+      <c r="H61" t="s">
         <v>8</v>
       </c>
-      <c r="I59" t="s">
+      <c r="I61" t="s">
         <v>17</v>
       </c>
-      <c r="J59" t="s">
+      <c r="J61" t="s">
         <v>18</v>
       </c>
-      <c r="K59" t="s">
+      <c r="K61" t="s">
         <v>19</v>
       </c>
-      <c r="L59" t="s">
+      <c r="L61" t="s">
         <v>29</v>
       </c>
-      <c r="M59" t="s">
+      <c r="M61" t="s">
         <v>27</v>
       </c>
-      <c r="N59" t="s">
+      <c r="N61" t="s">
         <v>23</v>
       </c>
-      <c r="O59" t="s">
+      <c r="O61" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A60">
-        <v>10617236</v>
-      </c>
-      <c r="B60">
-        <v>180</v>
-      </c>
-      <c r="C60">
-        <v>0.71</v>
-      </c>
-      <c r="D60" s="2">
-        <v>120</v>
-      </c>
-      <c r="E60" s="2">
-        <v>0</v>
-      </c>
-      <c r="F60" t="s">
-        <v>20</v>
-      </c>
-      <c r="G60">
-        <v>2</v>
-      </c>
-      <c r="H60" t="s">
-        <v>21</v>
-      </c>
-      <c r="I60">
-        <v>192</v>
-      </c>
-      <c r="J60">
-        <f>129*2</f>
-        <v>258</v>
-      </c>
-      <c r="K60">
-        <v>160</v>
-      </c>
-      <c r="L60" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M60">
-        <v>96</v>
-      </c>
-      <c r="N60" t="s">
-        <v>28</v>
-      </c>
-      <c r="O60" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A61">
-        <v>10622304</v>
-      </c>
-      <c r="B61">
-        <v>180</v>
-      </c>
-      <c r="C61">
-        <v>0.71</v>
-      </c>
-      <c r="D61" s="2">
-        <v>480</v>
-      </c>
-      <c r="E61" s="2">
-        <v>0</v>
-      </c>
-      <c r="F61" t="s">
-        <v>20</v>
-      </c>
-      <c r="G61">
-        <v>2</v>
-      </c>
-      <c r="H61" t="s">
-        <v>21</v>
-      </c>
-      <c r="I61">
-        <v>192</v>
-      </c>
-      <c r="J61">
-        <f>129*2</f>
-        <v>258</v>
-      </c>
-      <c r="K61">
-        <v>160</v>
-      </c>
-      <c r="L61" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M61">
-        <v>96</v>
-      </c>
-      <c r="N61" t="s">
-        <v>28</v>
-      </c>
-      <c r="O61" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A62">
-        <v>10622305</v>
+        <v>10617236</v>
       </c>
       <c r="B62">
         <v>180</v>
@@ -2766,7 +2729,7 @@
         <v>0.71</v>
       </c>
       <c r="D62" s="2">
-        <v>960</v>
+        <v>120</v>
       </c>
       <c r="E62" s="2">
         <v>0</v>
@@ -2800,6 +2763,102 @@
         <v>28</v>
       </c>
       <c r="O62" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A63">
+        <v>10622304</v>
+      </c>
+      <c r="B63">
+        <v>180</v>
+      </c>
+      <c r="C63">
+        <v>0.71</v>
+      </c>
+      <c r="D63" s="2">
+        <v>480</v>
+      </c>
+      <c r="E63" s="2">
+        <v>0</v>
+      </c>
+      <c r="F63" t="s">
+        <v>20</v>
+      </c>
+      <c r="G63">
+        <v>2</v>
+      </c>
+      <c r="H63" t="s">
+        <v>21</v>
+      </c>
+      <c r="I63">
+        <v>192</v>
+      </c>
+      <c r="J63">
+        <f>129*2</f>
+        <v>258</v>
+      </c>
+      <c r="K63">
+        <v>160</v>
+      </c>
+      <c r="L63" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M63">
+        <v>96</v>
+      </c>
+      <c r="N63" t="s">
+        <v>28</v>
+      </c>
+      <c r="O63" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A64">
+        <v>10622305</v>
+      </c>
+      <c r="B64">
+        <v>180</v>
+      </c>
+      <c r="C64">
+        <v>0.71</v>
+      </c>
+      <c r="D64" s="2">
+        <v>960</v>
+      </c>
+      <c r="E64" s="2">
+        <v>0</v>
+      </c>
+      <c r="F64" t="s">
+        <v>20</v>
+      </c>
+      <c r="G64">
+        <v>2</v>
+      </c>
+      <c r="H64" t="s">
+        <v>21</v>
+      </c>
+      <c r="I64">
+        <v>192</v>
+      </c>
+      <c r="J64">
+        <f>129*2</f>
+        <v>258</v>
+      </c>
+      <c r="K64">
+        <v>160</v>
+      </c>
+      <c r="L64" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M64">
+        <v>96</v>
+      </c>
+      <c r="N64" t="s">
+        <v>28</v>
+      </c>
+      <c r="O64" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update spanwise heterogeneous heating
</commit_message>
<xml_diff>
--- a/case_number_20250816.xlsx
+++ b/case_number_20250816.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chang\Nutstore\1\Nutstore\Workspace\convection_time_varying_T\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0F3E3A-F381-412F-825F-1611D1715BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F455EE-2DCE-47A2-8BE1-3847859CF534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="68">
   <si>
     <t>omega</t>
   </si>
@@ -192,9 +192,6 @@
     <t>bigmem</t>
   </si>
   <si>
-    <t>Below: with oscillating pressure gradient: continue from 10424250, t=100 of fully developed turbulence</t>
-  </si>
-  <si>
     <t>Ri_tau</t>
   </si>
   <si>
@@ -208,13 +205,49 @@
   </si>
   <si>
     <t>continue at t=4 from 10611110</t>
+  </si>
+  <si>
+    <t>Below: Add stably stratification (Total T formulation), without oscillating pressure gradient: continue from 10424250, t=100 of fully developed turbulence</t>
+  </si>
+  <si>
+    <t>Below: Add stable stratification (T fluctuation formulation), without oscillating pressure gradient: continue from 10424250, t=100 of fully developed turbulence</t>
+  </si>
+  <si>
+    <t>Final Time</t>
+  </si>
+  <si>
+    <t>Continuation after power outage</t>
+  </si>
+  <si>
+    <t>Continuation from</t>
+  </si>
+  <si>
+    <t>Final time</t>
+  </si>
+  <si>
+    <t>continue at t=20 from 10642100</t>
+  </si>
+  <si>
+    <t>5 days</t>
+  </si>
+  <si>
+    <t>continue at t=23 from 10758655</t>
+  </si>
+  <si>
+    <t>99 continue from unstratified channel</t>
+  </si>
+  <si>
+    <t>Initial time</t>
+  </si>
+  <si>
+    <t>-------</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,8 +255,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,6 +273,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -249,11 +295,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,10 +750,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0792B6-F3DE-44AA-920E-7B8294731BF8}">
-  <dimension ref="A1:Q64"/>
+  <dimension ref="A1:R79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1011,7 +1061,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L8" s="1"/>
     </row>
@@ -1119,7 +1169,7 @@
         <v>49</v>
       </c>
       <c r="P13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.5">
@@ -1169,23 +1219,112 @@
         <v>47</v>
       </c>
       <c r="Q14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="L15" s="1"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A17" t="s">
+      <c r="A15">
+        <v>10758655</v>
+      </c>
+      <c r="B15">
+        <v>395</v>
+      </c>
+      <c r="C15">
+        <v>0.71</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15">
+        <v>256</v>
+      </c>
+      <c r="J15">
+        <v>416</v>
+      </c>
+      <c r="K15">
+        <v>240</v>
+      </c>
+      <c r="L15" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="M15">
+        <v>104</v>
+      </c>
+      <c r="N15" t="s">
+        <v>50</v>
+      </c>
+      <c r="O15" t="s">
+        <v>49</v>
+      </c>
+      <c r="P15" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="A16">
+        <v>10779727</v>
+      </c>
+      <c r="B16">
+        <v>395</v>
+      </c>
+      <c r="C16">
+        <v>0.71</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16">
+        <v>256</v>
+      </c>
+      <c r="J16">
+        <v>416</v>
+      </c>
+      <c r="K16">
+        <v>240</v>
+      </c>
+      <c r="L16" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="M16">
+        <v>104</v>
+      </c>
+      <c r="N16" t="s">
+        <v>50</v>
+      </c>
+      <c r="O16" t="s">
+        <v>49</v>
+      </c>
+      <c r="P16" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A18" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="D18">
-        <v>0.1</v>
-      </c>
-      <c r="E18">
-        <v>0.02</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.5">
@@ -1193,7 +1332,7 @@
         <v>0.1</v>
       </c>
       <c r="E19">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.5">
@@ -1201,65 +1340,25 @@
         <v>0.1</v>
       </c>
       <c r="E20">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="D21">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="B22">
+      <c r="E21">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="B23">
         <v>150</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A24">
-        <v>10525261</v>
-      </c>
-      <c r="B24">
-        <v>180</v>
-      </c>
-      <c r="C24">
-        <v>0.71</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="E24" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24">
-        <v>2</v>
-      </c>
-      <c r="H24" t="s">
-        <v>21</v>
-      </c>
-      <c r="I24">
-        <v>192</v>
-      </c>
-      <c r="J24">
-        <f>129*2</f>
-        <v>258</v>
-      </c>
-      <c r="K24">
-        <v>160</v>
-      </c>
-      <c r="L24" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M24">
-        <v>96</v>
-      </c>
-      <c r="N24" t="s">
-        <v>28</v>
-      </c>
-      <c r="O24" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A25">
-        <v>10476429</v>
+        <v>10525261</v>
       </c>
       <c r="B25">
         <v>180</v>
@@ -1271,7 +1370,7 @@
         <v>0.1</v>
       </c>
       <c r="E25" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F25" t="s">
         <v>20</v>
@@ -1306,8 +1405,8 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A26">
-        <v>10478562</v>
+      <c r="A26" s="4">
+        <v>10476429</v>
       </c>
       <c r="B26">
         <v>180</v>
@@ -1319,22 +1418,22 @@
         <v>0.1</v>
       </c>
       <c r="E26" s="2">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="F26" t="s">
         <v>20</v>
       </c>
       <c r="G26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H26" t="s">
         <v>21</v>
       </c>
       <c r="I26">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J26">
-        <f t="shared" ref="J26:J57" si="0">129*2</f>
+        <f>129*2</f>
         <v>258</v>
       </c>
       <c r="K26">
@@ -1355,7 +1454,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A27">
-        <v>10478905</v>
+        <v>10478562</v>
       </c>
       <c r="B27">
         <v>180</v>
@@ -1367,22 +1466,22 @@
         <v>0.1</v>
       </c>
       <c r="E27" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F27" t="s">
         <v>20</v>
       </c>
       <c r="G27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H27" t="s">
         <v>21</v>
       </c>
       <c r="I27">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J27">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J27:J58" si="0">129*2</f>
         <v>258</v>
       </c>
       <c r="K27">
@@ -1403,7 +1502,7 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A28">
-        <v>10478910</v>
+        <v>10478905</v>
       </c>
       <c r="B28">
         <v>180</v>
@@ -1415,19 +1514,19 @@
         <v>0.1</v>
       </c>
       <c r="E28" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="s">
         <v>20</v>
       </c>
       <c r="G28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H28" t="s">
         <v>21</v>
       </c>
       <c r="I28">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J28">
         <f t="shared" si="0"/>
@@ -1451,7 +1550,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A29">
-        <v>10478912</v>
+        <v>10478910</v>
       </c>
       <c r="B29">
         <v>180</v>
@@ -1463,19 +1562,19 @@
         <v>0.1</v>
       </c>
       <c r="E29" s="2">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29">
         <v>5</v>
       </c>
-      <c r="F29" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29">
-        <v>6</v>
-      </c>
       <c r="H29" t="s">
         <v>21</v>
       </c>
       <c r="I29">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J29">
         <f t="shared" si="0"/>
@@ -1498,61 +1597,61 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="L30" s="1"/>
+      <c r="A30">
+        <v>10478912</v>
+      </c>
+      <c r="B30">
+        <v>180</v>
+      </c>
+      <c r="C30">
+        <v>0.71</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E30" s="2">
+        <v>5</v>
+      </c>
+      <c r="F30" t="s">
+        <v>20</v>
+      </c>
+      <c r="G30">
+        <v>6</v>
+      </c>
+      <c r="H30" t="s">
+        <v>21</v>
+      </c>
+      <c r="I30">
+        <v>196</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K30">
+        <v>160</v>
+      </c>
+      <c r="L30" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M30">
+        <v>96</v>
+      </c>
+      <c r="N30" t="s">
+        <v>28</v>
+      </c>
+      <c r="O30" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A31">
-        <v>10526147</v>
-      </c>
-      <c r="B31">
-        <v>180</v>
-      </c>
-      <c r="C31">
-        <v>0.71</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="E31" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F31" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31">
-        <v>7</v>
-      </c>
-      <c r="H31" t="s">
-        <v>21</v>
-      </c>
-      <c r="I31">
-        <v>197</v>
-      </c>
-      <c r="J31">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="K31">
-        <v>160</v>
-      </c>
-      <c r="L31" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M31">
-        <v>96</v>
-      </c>
-      <c r="N31" t="s">
-        <v>28</v>
-      </c>
-      <c r="O31" t="s">
-        <v>46</v>
-      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A32">
-        <v>10479023</v>
+        <v>10526147</v>
       </c>
       <c r="B32">
         <v>180</v>
@@ -1564,7 +1663,7 @@
         <v>0.2</v>
       </c>
       <c r="E32" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F32" t="s">
         <v>20</v>
@@ -1600,7 +1699,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A33">
-        <v>10479256</v>
+        <v>10479023</v>
       </c>
       <c r="B33">
         <v>180</v>
@@ -1612,19 +1711,19 @@
         <v>0.2</v>
       </c>
       <c r="E33" s="2">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="F33" t="s">
         <v>20</v>
       </c>
       <c r="G33">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H33" t="s">
         <v>21</v>
       </c>
       <c r="I33">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
@@ -1648,7 +1747,7 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A34">
-        <v>10481244</v>
+        <v>10479256</v>
       </c>
       <c r="B34">
         <v>180</v>
@@ -1660,19 +1759,19 @@
         <v>0.2</v>
       </c>
       <c r="E34" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F34" t="s">
         <v>20</v>
       </c>
       <c r="G34">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H34" t="s">
         <v>21</v>
       </c>
       <c r="I34">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
@@ -1696,7 +1795,7 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A35">
-        <v>10481262</v>
+        <v>10481244</v>
       </c>
       <c r="B35">
         <v>180</v>
@@ -1708,19 +1807,19 @@
         <v>0.2</v>
       </c>
       <c r="E35" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="s">
         <v>20</v>
       </c>
       <c r="G35">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H35" t="s">
         <v>21</v>
       </c>
       <c r="I35">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J35">
         <f t="shared" si="0"/>
@@ -1744,7 +1843,7 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A36">
-        <v>10481790</v>
+        <v>10481262</v>
       </c>
       <c r="B36">
         <v>180</v>
@@ -1756,19 +1855,19 @@
         <v>0.2</v>
       </c>
       <c r="E36" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F36" t="s">
         <v>20</v>
       </c>
       <c r="G36">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H36" t="s">
         <v>21</v>
       </c>
       <c r="I36">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J36">
         <f t="shared" si="0"/>
@@ -1791,61 +1890,61 @@
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="L37" s="1"/>
+      <c r="A37">
+        <v>10481790</v>
+      </c>
+      <c r="B37">
+        <v>180</v>
+      </c>
+      <c r="C37">
+        <v>0.71</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E37" s="2">
+        <v>5</v>
+      </c>
+      <c r="F37" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37">
+        <v>11</v>
+      </c>
+      <c r="H37" t="s">
+        <v>21</v>
+      </c>
+      <c r="I37">
+        <v>201</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K37">
+        <v>160</v>
+      </c>
+      <c r="L37" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M37">
+        <v>96</v>
+      </c>
+      <c r="N37" t="s">
+        <v>28</v>
+      </c>
+      <c r="O37" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A38">
-        <v>10526152</v>
-      </c>
-      <c r="B38">
-        <v>180</v>
-      </c>
-      <c r="C38">
-        <v>0.71</v>
-      </c>
-      <c r="D38" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="E38" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F38" t="s">
-        <v>20</v>
-      </c>
-      <c r="G38">
-        <v>12</v>
-      </c>
-      <c r="H38" t="s">
-        <v>21</v>
-      </c>
-      <c r="I38">
-        <v>202</v>
-      </c>
-      <c r="J38">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="K38">
-        <v>160</v>
-      </c>
-      <c r="L38" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M38">
-        <v>96</v>
-      </c>
-      <c r="N38" t="s">
-        <v>28</v>
-      </c>
-      <c r="O38" t="s">
-        <v>46</v>
-      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="L38" s="1"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A39">
-        <v>10482459</v>
+        <v>10526152</v>
       </c>
       <c r="B39">
         <v>180</v>
@@ -1857,7 +1956,7 @@
         <v>0.3</v>
       </c>
       <c r="E39" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F39" t="s">
         <v>20</v>
@@ -1893,7 +1992,7 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A40">
-        <v>10484952</v>
+        <v>10482459</v>
       </c>
       <c r="B40">
         <v>180</v>
@@ -1905,19 +2004,19 @@
         <v>0.3</v>
       </c>
       <c r="E40" s="2">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="F40" t="s">
         <v>20</v>
       </c>
       <c r="G40">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H40" t="s">
         <v>21</v>
       </c>
       <c r="I40">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
@@ -1941,7 +2040,7 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A41">
-        <v>10490537</v>
+        <v>10484952</v>
       </c>
       <c r="B41">
         <v>180</v>
@@ -1953,19 +2052,19 @@
         <v>0.3</v>
       </c>
       <c r="E41" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F41" t="s">
         <v>20</v>
       </c>
       <c r="G41">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H41" t="s">
         <v>21</v>
       </c>
       <c r="I41">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
@@ -1989,7 +2088,7 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A42">
-        <v>10500013</v>
+        <v>10490537</v>
       </c>
       <c r="B42">
         <v>180</v>
@@ -2001,19 +2100,19 @@
         <v>0.3</v>
       </c>
       <c r="E42" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="s">
         <v>20</v>
       </c>
       <c r="G42">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H42" t="s">
         <v>21</v>
       </c>
       <c r="I42">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
@@ -2037,7 +2136,7 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A43">
-        <v>10500017</v>
+        <v>10500013</v>
       </c>
       <c r="B43">
         <v>180</v>
@@ -2049,19 +2148,19 @@
         <v>0.3</v>
       </c>
       <c r="E43" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F43" t="s">
         <v>20</v>
       </c>
       <c r="G43">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H43" t="s">
         <v>21</v>
       </c>
       <c r="I43">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
@@ -2084,61 +2183,61 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="L44" s="1"/>
+      <c r="A44">
+        <v>10500017</v>
+      </c>
+      <c r="B44">
+        <v>180</v>
+      </c>
+      <c r="C44">
+        <v>0.71</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E44" s="2">
+        <v>5</v>
+      </c>
+      <c r="F44" t="s">
+        <v>20</v>
+      </c>
+      <c r="G44">
+        <v>16</v>
+      </c>
+      <c r="H44" t="s">
+        <v>21</v>
+      </c>
+      <c r="I44">
+        <v>206</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K44">
+        <v>160</v>
+      </c>
+      <c r="L44" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M44">
+        <v>96</v>
+      </c>
+      <c r="N44" t="s">
+        <v>28</v>
+      </c>
+      <c r="O44" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A45">
-        <v>10526156</v>
-      </c>
-      <c r="B45">
-        <v>180</v>
-      </c>
-      <c r="C45">
-        <v>0.71</v>
-      </c>
-      <c r="D45" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="E45" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F45" t="s">
-        <v>20</v>
-      </c>
-      <c r="G45">
-        <v>17</v>
-      </c>
-      <c r="H45" t="s">
-        <v>21</v>
-      </c>
-      <c r="I45">
-        <v>207</v>
-      </c>
-      <c r="J45">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="K45">
-        <v>160</v>
-      </c>
-      <c r="L45" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M45">
-        <v>96</v>
-      </c>
-      <c r="N45" t="s">
-        <v>28</v>
-      </c>
-      <c r="O45" t="s">
-        <v>46</v>
-      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="L45" s="1"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A46">
-        <v>10500654</v>
+        <v>10526156</v>
       </c>
       <c r="B46">
         <v>180</v>
@@ -2150,7 +2249,7 @@
         <v>0.4</v>
       </c>
       <c r="E46" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F46" t="s">
         <v>20</v>
@@ -2186,7 +2285,7 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A47">
-        <v>10501196</v>
+        <v>10500654</v>
       </c>
       <c r="B47">
         <v>180</v>
@@ -2198,19 +2297,19 @@
         <v>0.4</v>
       </c>
       <c r="E47" s="2">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="F47" t="s">
         <v>20</v>
       </c>
       <c r="G47">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H47" t="s">
         <v>21</v>
       </c>
       <c r="I47">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
@@ -2234,7 +2333,7 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A48">
-        <v>10501212</v>
+        <v>10501196</v>
       </c>
       <c r="B48">
         <v>180</v>
@@ -2246,19 +2345,19 @@
         <v>0.4</v>
       </c>
       <c r="E48" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F48" t="s">
         <v>20</v>
       </c>
       <c r="G48">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H48" t="s">
         <v>21</v>
       </c>
       <c r="I48">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
@@ -2282,7 +2381,7 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A49">
-        <v>10501276</v>
+        <v>10501212</v>
       </c>
       <c r="B49">
         <v>180</v>
@@ -2294,19 +2393,19 @@
         <v>0.4</v>
       </c>
       <c r="E49" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="s">
         <v>20</v>
       </c>
       <c r="G49">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H49" t="s">
         <v>21</v>
       </c>
       <c r="I49">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
@@ -2330,7 +2429,7 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A50">
-        <v>10507648</v>
+        <v>10501276</v>
       </c>
       <c r="B50">
         <v>180</v>
@@ -2342,19 +2441,19 @@
         <v>0.4</v>
       </c>
       <c r="E50" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F50" t="s">
         <v>20</v>
       </c>
       <c r="G50">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H50" t="s">
         <v>21</v>
       </c>
       <c r="I50">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
@@ -2377,61 +2476,61 @@
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="L51" s="1"/>
+      <c r="A51">
+        <v>10507648</v>
+      </c>
+      <c r="B51">
+        <v>180</v>
+      </c>
+      <c r="C51">
+        <v>0.71</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="E51" s="2">
+        <v>5</v>
+      </c>
+      <c r="F51" t="s">
+        <v>20</v>
+      </c>
+      <c r="G51">
+        <v>21</v>
+      </c>
+      <c r="H51" t="s">
+        <v>21</v>
+      </c>
+      <c r="I51">
+        <v>211</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K51">
+        <v>160</v>
+      </c>
+      <c r="L51" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M51">
+        <v>96</v>
+      </c>
+      <c r="N51" t="s">
+        <v>28</v>
+      </c>
+      <c r="O51" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A52">
-        <v>10526159</v>
-      </c>
-      <c r="B52">
-        <v>180</v>
-      </c>
-      <c r="C52">
-        <v>0.71</v>
-      </c>
-      <c r="D52" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E52" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F52" t="s">
-        <v>20</v>
-      </c>
-      <c r="G52">
-        <v>17</v>
-      </c>
-      <c r="H52" t="s">
-        <v>21</v>
-      </c>
-      <c r="I52">
-        <v>207</v>
-      </c>
-      <c r="J52">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="K52">
-        <v>160</v>
-      </c>
-      <c r="L52" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M52">
-        <v>96</v>
-      </c>
-      <c r="N52" t="s">
-        <v>28</v>
-      </c>
-      <c r="O52" t="s">
-        <v>46</v>
-      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="L52" s="1"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A53">
-        <v>10512815</v>
+        <v>10526159</v>
       </c>
       <c r="B53">
         <v>180</v>
@@ -2443,7 +2542,7 @@
         <v>0.5</v>
       </c>
       <c r="E53" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F53" t="s">
         <v>20</v>
@@ -2479,7 +2578,7 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A54">
-        <v>10512816</v>
+        <v>10512815</v>
       </c>
       <c r="B54">
         <v>180</v>
@@ -2491,19 +2590,19 @@
         <v>0.5</v>
       </c>
       <c r="E54" s="2">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="F54" t="s">
         <v>20</v>
       </c>
       <c r="G54">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H54" t="s">
         <v>21</v>
       </c>
       <c r="I54">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
@@ -2527,7 +2626,7 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A55">
-        <v>10512818</v>
+        <v>10512816</v>
       </c>
       <c r="B55">
         <v>180</v>
@@ -2539,19 +2638,19 @@
         <v>0.5</v>
       </c>
       <c r="E55" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F55" t="s">
         <v>20</v>
       </c>
       <c r="G55">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H55" t="s">
         <v>21</v>
       </c>
       <c r="I55">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J55">
         <f t="shared" si="0"/>
@@ -2575,7 +2674,7 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A56">
-        <v>10513758</v>
+        <v>10512818</v>
       </c>
       <c r="B56">
         <v>180</v>
@@ -2587,19 +2686,19 @@
         <v>0.5</v>
       </c>
       <c r="E56" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="s">
         <v>20</v>
       </c>
       <c r="G56">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H56" t="s">
         <v>21</v>
       </c>
       <c r="I56">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J56">
         <f t="shared" si="0"/>
@@ -2623,7 +2722,7 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A57">
-        <v>10514336</v>
+        <v>10513758</v>
       </c>
       <c r="B57">
         <v>180</v>
@@ -2635,19 +2734,19 @@
         <v>0.5</v>
       </c>
       <c r="E57" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F57" t="s">
         <v>20</v>
       </c>
       <c r="G57">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H57" t="s">
         <v>21</v>
       </c>
       <c r="I57">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J57">
         <f t="shared" si="0"/>
@@ -2669,106 +2768,106 @@
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A60" t="s">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A58">
+        <v>10514336</v>
+      </c>
+      <c r="B58">
+        <v>180</v>
+      </c>
+      <c r="C58">
+        <v>0.71</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E58" s="2">
+        <v>5</v>
+      </c>
+      <c r="F58" t="s">
+        <v>20</v>
+      </c>
+      <c r="G58">
+        <v>21</v>
+      </c>
+      <c r="H58" t="s">
+        <v>21</v>
+      </c>
+      <c r="I58">
+        <v>211</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="K58">
+        <v>160</v>
+      </c>
+      <c r="L58" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M58">
+        <v>96</v>
+      </c>
+      <c r="N58" t="s">
+        <v>28</v>
+      </c>
+      <c r="O58" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A61" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="B62" t="s">
+        <v>16</v>
+      </c>
+      <c r="C62" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="B61" t="s">
-        <v>16</v>
-      </c>
-      <c r="C61" t="s">
-        <v>4</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="E62" t="s">
         <v>52</v>
       </c>
-      <c r="E61" t="s">
-        <v>53</v>
-      </c>
-      <c r="F61" t="s">
+      <c r="F62" t="s">
         <v>5</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G62" t="s">
         <v>7</v>
       </c>
-      <c r="H61" t="s">
+      <c r="H62" t="s">
         <v>8</v>
       </c>
-      <c r="I61" t="s">
+      <c r="I62" t="s">
         <v>17</v>
       </c>
-      <c r="J61" t="s">
+      <c r="J62" t="s">
         <v>18</v>
       </c>
-      <c r="K61" t="s">
+      <c r="K62" t="s">
         <v>19</v>
       </c>
-      <c r="L61" t="s">
+      <c r="L62" t="s">
         <v>29</v>
       </c>
-      <c r="M61" t="s">
+      <c r="M62" t="s">
         <v>27</v>
       </c>
-      <c r="N61" t="s">
+      <c r="N62" t="s">
         <v>23</v>
       </c>
-      <c r="O61" t="s">
+      <c r="O62" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A62">
-        <v>10617236</v>
-      </c>
-      <c r="B62">
-        <v>180</v>
-      </c>
-      <c r="C62">
-        <v>0.71</v>
-      </c>
-      <c r="D62" s="2">
-        <v>120</v>
-      </c>
-      <c r="E62" s="2">
-        <v>0</v>
-      </c>
-      <c r="F62" t="s">
-        <v>20</v>
-      </c>
-      <c r="G62">
-        <v>2</v>
-      </c>
-      <c r="H62" t="s">
-        <v>21</v>
-      </c>
-      <c r="I62">
-        <v>192</v>
-      </c>
-      <c r="J62">
-        <f>129*2</f>
-        <v>258</v>
-      </c>
-      <c r="K62">
-        <v>160</v>
-      </c>
-      <c r="L62" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="M62">
-        <v>96</v>
-      </c>
-      <c r="N62" t="s">
-        <v>28</v>
-      </c>
-      <c r="O62" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A63">
-        <v>10622304</v>
+        <v>10617236</v>
       </c>
       <c r="B63">
         <v>180</v>
@@ -2777,7 +2876,7 @@
         <v>0.71</v>
       </c>
       <c r="D63" s="2">
-        <v>480</v>
+        <v>120</v>
       </c>
       <c r="E63" s="2">
         <v>0</v>
@@ -2816,7 +2915,7 @@
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A64">
-        <v>10622305</v>
+        <v>10622304</v>
       </c>
       <c r="B64">
         <v>180</v>
@@ -2825,7 +2924,7 @@
         <v>0.71</v>
       </c>
       <c r="D64" s="2">
-        <v>960</v>
+        <v>480</v>
       </c>
       <c r="E64" s="2">
         <v>0</v>
@@ -2860,6 +2959,553 @@
       </c>
       <c r="O64" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A65">
+        <v>10622305</v>
+      </c>
+      <c r="B65">
+        <v>180</v>
+      </c>
+      <c r="C65">
+        <v>0.71</v>
+      </c>
+      <c r="D65" s="2">
+        <v>960</v>
+      </c>
+      <c r="E65" s="2">
+        <v>0</v>
+      </c>
+      <c r="F65" t="s">
+        <v>20</v>
+      </c>
+      <c r="G65">
+        <v>2</v>
+      </c>
+      <c r="H65" t="s">
+        <v>21</v>
+      </c>
+      <c r="I65">
+        <v>192</v>
+      </c>
+      <c r="J65">
+        <f>129*2</f>
+        <v>258</v>
+      </c>
+      <c r="K65">
+        <v>160</v>
+      </c>
+      <c r="L65" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M65">
+        <v>96</v>
+      </c>
+      <c r="N65" t="s">
+        <v>28</v>
+      </c>
+      <c r="O65" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A67" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="B68" t="s">
+        <v>16</v>
+      </c>
+      <c r="C68" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68" t="s">
+        <v>51</v>
+      </c>
+      <c r="E68" t="s">
+        <v>52</v>
+      </c>
+      <c r="F68" t="s">
+        <v>5</v>
+      </c>
+      <c r="G68" t="s">
+        <v>7</v>
+      </c>
+      <c r="H68" t="s">
+        <v>8</v>
+      </c>
+      <c r="I68" t="s">
+        <v>17</v>
+      </c>
+      <c r="J68" t="s">
+        <v>18</v>
+      </c>
+      <c r="K68" t="s">
+        <v>19</v>
+      </c>
+      <c r="L68" t="s">
+        <v>29</v>
+      </c>
+      <c r="M68" t="s">
+        <v>27</v>
+      </c>
+      <c r="N68" t="s">
+        <v>23</v>
+      </c>
+      <c r="O68" t="s">
+        <v>25</v>
+      </c>
+      <c r="P68" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A69">
+        <v>10659257</v>
+      </c>
+      <c r="B69">
+        <v>180</v>
+      </c>
+      <c r="C69">
+        <v>0.71</v>
+      </c>
+      <c r="D69" s="2">
+        <v>120</v>
+      </c>
+      <c r="E69" s="2">
+        <v>0</v>
+      </c>
+      <c r="F69" t="s">
+        <v>20</v>
+      </c>
+      <c r="G69">
+        <v>2</v>
+      </c>
+      <c r="H69" t="s">
+        <v>21</v>
+      </c>
+      <c r="I69">
+        <v>192</v>
+      </c>
+      <c r="J69">
+        <f>129*2</f>
+        <v>258</v>
+      </c>
+      <c r="K69">
+        <v>160</v>
+      </c>
+      <c r="L69" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M69">
+        <v>96</v>
+      </c>
+      <c r="N69" t="s">
+        <v>28</v>
+      </c>
+      <c r="O69" t="s">
+        <v>46</v>
+      </c>
+      <c r="P69">
+        <v>148.19</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A70">
+        <v>10659450</v>
+      </c>
+      <c r="B70">
+        <v>180</v>
+      </c>
+      <c r="C70">
+        <v>0.71</v>
+      </c>
+      <c r="D70" s="2">
+        <v>480</v>
+      </c>
+      <c r="E70" s="2">
+        <v>0</v>
+      </c>
+      <c r="F70" t="s">
+        <v>20</v>
+      </c>
+      <c r="G70">
+        <v>2</v>
+      </c>
+      <c r="H70" t="s">
+        <v>21</v>
+      </c>
+      <c r="I70">
+        <v>192</v>
+      </c>
+      <c r="J70">
+        <f>129*2</f>
+        <v>258</v>
+      </c>
+      <c r="K70">
+        <v>160</v>
+      </c>
+      <c r="L70" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M70">
+        <v>96</v>
+      </c>
+      <c r="N70" t="s">
+        <v>28</v>
+      </c>
+      <c r="O70" t="s">
+        <v>46</v>
+      </c>
+      <c r="P70">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A71">
+        <v>10660444</v>
+      </c>
+      <c r="B71">
+        <v>180</v>
+      </c>
+      <c r="C71">
+        <v>0.71</v>
+      </c>
+      <c r="D71" s="2">
+        <v>960</v>
+      </c>
+      <c r="E71" s="2">
+        <v>0</v>
+      </c>
+      <c r="F71" t="s">
+        <v>20</v>
+      </c>
+      <c r="G71">
+        <v>2</v>
+      </c>
+      <c r="H71" t="s">
+        <v>21</v>
+      </c>
+      <c r="I71">
+        <v>192</v>
+      </c>
+      <c r="J71">
+        <f>129*2</f>
+        <v>258</v>
+      </c>
+      <c r="K71">
+        <v>160</v>
+      </c>
+      <c r="L71" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M71">
+        <v>96</v>
+      </c>
+      <c r="N71" t="s">
+        <v>28</v>
+      </c>
+      <c r="O71" t="s">
+        <v>46</v>
+      </c>
+      <c r="P71">
+        <v>103.97</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A73" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="B74" t="s">
+        <v>16</v>
+      </c>
+      <c r="C74" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74" t="s">
+        <v>51</v>
+      </c>
+      <c r="E74" t="s">
+        <v>52</v>
+      </c>
+      <c r="F74" t="s">
+        <v>5</v>
+      </c>
+      <c r="G74" t="s">
+        <v>7</v>
+      </c>
+      <c r="H74" t="s">
+        <v>8</v>
+      </c>
+      <c r="I74" t="s">
+        <v>17</v>
+      </c>
+      <c r="J74" t="s">
+        <v>18</v>
+      </c>
+      <c r="K74" t="s">
+        <v>19</v>
+      </c>
+      <c r="L74" t="s">
+        <v>29</v>
+      </c>
+      <c r="M74" t="s">
+        <v>27</v>
+      </c>
+      <c r="N74" t="s">
+        <v>23</v>
+      </c>
+      <c r="O74" t="s">
+        <v>25</v>
+      </c>
+      <c r="P74" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>60</v>
+      </c>
+      <c r="R74" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A75" s="5">
+        <v>10722660</v>
+      </c>
+      <c r="B75" s="5">
+        <v>180</v>
+      </c>
+      <c r="C75" s="5">
+        <v>0.71</v>
+      </c>
+      <c r="D75" s="5">
+        <v>120</v>
+      </c>
+      <c r="E75" s="5">
+        <v>0</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G75" s="5">
+        <v>2</v>
+      </c>
+      <c r="H75" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I75" s="5">
+        <v>192</v>
+      </c>
+      <c r="J75" s="5">
+        <f>129*2</f>
+        <v>258</v>
+      </c>
+      <c r="K75" s="5">
+        <v>160</v>
+      </c>
+      <c r="L75" s="6">
+        <v>1E-4</v>
+      </c>
+      <c r="M75" s="5">
+        <v>96</v>
+      </c>
+      <c r="N75" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O75" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="P75" s="5">
+        <v>244</v>
+      </c>
+      <c r="Q75" s="5">
+        <v>10659257</v>
+      </c>
+      <c r="R75" s="5">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A76">
+        <v>10778092</v>
+      </c>
+      <c r="B76">
+        <v>180</v>
+      </c>
+      <c r="C76">
+        <v>0.71</v>
+      </c>
+      <c r="D76" s="2">
+        <v>120</v>
+      </c>
+      <c r="E76" s="2">
+        <v>0</v>
+      </c>
+      <c r="F76" t="s">
+        <v>20</v>
+      </c>
+      <c r="G76">
+        <v>2</v>
+      </c>
+      <c r="H76" t="s">
+        <v>21</v>
+      </c>
+      <c r="I76">
+        <v>192</v>
+      </c>
+      <c r="J76">
+        <f>129*2</f>
+        <v>258</v>
+      </c>
+      <c r="K76">
+        <v>160</v>
+      </c>
+      <c r="L76" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M76">
+        <v>96</v>
+      </c>
+      <c r="N76" t="s">
+        <v>28</v>
+      </c>
+      <c r="O76" t="s">
+        <v>46</v>
+      </c>
+      <c r="P76">
+        <v>306</v>
+      </c>
+      <c r="Q76">
+        <v>10722660</v>
+      </c>
+      <c r="R76">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="L77" s="1"/>
+    </row>
+    <row r="78" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A78" s="5">
+        <v>10758396</v>
+      </c>
+      <c r="B78" s="5">
+        <v>180</v>
+      </c>
+      <c r="C78" s="5">
+        <v>0.71</v>
+      </c>
+      <c r="D78" s="5">
+        <v>480</v>
+      </c>
+      <c r="E78" s="5">
+        <v>0</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G78" s="5">
+        <v>2</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I78" s="5">
+        <v>192</v>
+      </c>
+      <c r="J78" s="5">
+        <f>129*2</f>
+        <v>258</v>
+      </c>
+      <c r="K78" s="5">
+        <v>160</v>
+      </c>
+      <c r="L78" s="6">
+        <v>1E-4</v>
+      </c>
+      <c r="M78" s="5">
+        <v>96</v>
+      </c>
+      <c r="N78" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O78" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="P78" s="5">
+        <v>203</v>
+      </c>
+      <c r="Q78" s="5">
+        <v>10659450</v>
+      </c>
+      <c r="R78" s="5">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A79" s="5">
+        <v>10819165</v>
+      </c>
+      <c r="B79" s="5">
+        <v>180</v>
+      </c>
+      <c r="C79" s="5">
+        <v>0.71</v>
+      </c>
+      <c r="D79" s="5">
+        <v>480</v>
+      </c>
+      <c r="E79" s="5">
+        <v>0</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G79" s="5">
+        <v>2</v>
+      </c>
+      <c r="H79" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I79" s="5">
+        <v>192</v>
+      </c>
+      <c r="J79" s="5">
+        <f>129*2</f>
+        <v>258</v>
+      </c>
+      <c r="K79" s="5">
+        <v>160</v>
+      </c>
+      <c r="L79" s="6">
+        <v>1E-4</v>
+      </c>
+      <c r="M79" s="5">
+        <v>96</v>
+      </c>
+      <c r="N79" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O79" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="P79" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q79" s="5">
+        <v>10758396</v>
+      </c>
+      <c r="R79" s="5">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update only compliant wall on one side
</commit_message>
<xml_diff>
--- a/case_number_20250816.xlsx
+++ b/case_number_20250816.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chang\Nutstore\1\Nutstore\Workspace\convection_time_varying_T\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1395A6-C8D9-4EEC-A55B-26E635F056AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5C7BFF-68FF-4EC3-9BD7-90E512AAADC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Turbulent convection NREL clust" sheetId="2" r:id="rId2"/>
+    <sheet name="compliant_wall" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="72">
   <si>
     <t>omega</t>
   </si>
@@ -244,6 +245,15 @@
   </si>
   <si>
     <t>-----</t>
+  </si>
+  <si>
+    <t>Cm</t>
+  </si>
+  <si>
+    <t>Cd</t>
+  </si>
+  <si>
+    <t>Ck</t>
   </si>
 </sst>
 </file>
@@ -593,12 +603,12 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="22.29296875" customWidth="1"/>
+    <col min="1" max="1" width="22.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -642,7 +652,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>16473707</v>
       </c>
@@ -683,7 +693,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>16473708</v>
       </c>
@@ -694,7 +704,7 @@
         <v>4.3718000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>16473709</v>
       </c>
@@ -705,7 +715,7 @@
         <v>6.5491000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>16473711</v>
       </c>
@@ -713,7 +723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>16473713</v>
       </c>
@@ -721,7 +731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>16473717</v>
       </c>
@@ -729,7 +739,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>16473719</v>
       </c>
@@ -737,7 +747,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>16473721</v>
       </c>
@@ -755,16 +765,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0792B6-F3DE-44AA-920E-7B8294731BF8}">
   <dimension ref="A1:R79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="31.29296875" customWidth="1"/>
+    <col min="1" max="1" width="31.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -817,7 +827,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>10249087</v>
       </c>
@@ -861,7 +871,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -912,7 +922,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>10336395</v>
       </c>
@@ -962,7 +972,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>10337407</v>
       </c>
@@ -1009,7 +1019,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>10473706</v>
       </c>
@@ -1059,16 +1069,16 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>53</v>
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2">
         <v>10629945</v>
       </c>
@@ -1116,19 +1126,19 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>48</v>
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>10611110</v>
       </c>
@@ -1175,7 +1185,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>10642100</v>
       </c>
@@ -1225,7 +1235,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>10758655</v>
       </c>
@@ -1275,7 +1285,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>10779727</v>
       </c>
@@ -1325,12 +1335,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="D19">
         <v>0.1</v>
       </c>
@@ -1338,7 +1348,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="D20">
         <v>0.1</v>
       </c>
@@ -1346,7 +1356,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="D21">
         <v>0.1</v>
       </c>
@@ -1354,12 +1364,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B23">
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>10525261</v>
       </c>
@@ -1407,7 +1417,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="4">
         <v>10476429</v>
       </c>
@@ -1455,7 +1465,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>10478562</v>
       </c>
@@ -1503,7 +1513,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>10478905</v>
       </c>
@@ -1551,7 +1561,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>10478910</v>
       </c>
@@ -1599,7 +1609,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>10478912</v>
       </c>
@@ -1647,12 +1657,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>10526147</v>
       </c>
@@ -1700,7 +1710,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>10479023</v>
       </c>
@@ -1748,7 +1758,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>10479256</v>
       </c>
@@ -1796,7 +1806,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>10481244</v>
       </c>
@@ -1844,7 +1854,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>10481262</v>
       </c>
@@ -1892,7 +1902,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>10481790</v>
       </c>
@@ -1940,12 +1950,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="L38" s="1"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <v>10526152</v>
       </c>
@@ -1993,7 +2003,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>10482459</v>
       </c>
@@ -2041,7 +2051,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>10484952</v>
       </c>
@@ -2089,7 +2099,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>10490537</v>
       </c>
@@ -2137,7 +2147,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <v>10500013</v>
       </c>
@@ -2185,7 +2195,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>10500017</v>
       </c>
@@ -2233,12 +2243,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="L45" s="1"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <v>10526156</v>
       </c>
@@ -2286,7 +2296,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
         <v>10500654</v>
       </c>
@@ -2334,7 +2344,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <v>10501196</v>
       </c>
@@ -2382,7 +2392,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
         <v>10501212</v>
       </c>
@@ -2430,7 +2440,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <v>10501276</v>
       </c>
@@ -2478,7 +2488,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
         <v>10507648</v>
       </c>
@@ -2526,12 +2536,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="L52" s="1"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
         <v>10526159</v>
       </c>
@@ -2579,7 +2589,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
         <v>10512815</v>
       </c>
@@ -2627,7 +2637,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
         <v>10512816</v>
       </c>
@@ -2675,7 +2685,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
         <v>10512818</v>
       </c>
@@ -2723,7 +2733,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
         <v>10513758</v>
       </c>
@@ -2771,7 +2781,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
         <v>10514336</v>
       </c>
@@ -2819,12 +2829,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B62" t="s">
         <v>16</v>
       </c>
@@ -2868,7 +2878,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
         <v>10617236</v>
       </c>
@@ -2916,7 +2926,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
         <v>10622304</v>
       </c>
@@ -2964,7 +2974,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
         <v>10622305</v>
       </c>
@@ -3012,12 +3022,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="B68" t="s">
         <v>16</v>
       </c>
@@ -3064,7 +3074,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
         <v>10659257</v>
       </c>
@@ -3118,7 +3128,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
         <v>10659450</v>
       </c>
@@ -3169,7 +3179,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A71">
         <v>10660444</v>
       </c>
@@ -3220,12 +3230,12 @@
         <v>103.97</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="B74" t="s">
         <v>16</v>
       </c>
@@ -3278,7 +3288,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="75" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="5">
         <v>10722660</v>
       </c>
@@ -3335,7 +3345,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A76">
         <v>10778092</v>
       </c>
@@ -3392,12 +3402,12 @@
         <v>244</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
       <c r="L77" s="1"/>
     </row>
-    <row r="78" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="5">
         <v>10758396</v>
       </c>
@@ -3454,7 +3464,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="79" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="7" t="s">
         <v>68</v>
       </c>
@@ -3515,4 +3525,113 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89384A63-B630-4FD1-9C62-6B1553DE358B}">
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2">
+        <v>180</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>-2.93</v>
+      </c>
+      <c r="E2">
+        <v>28859</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2">
+        <v>192</v>
+      </c>
+      <c r="J2">
+        <v>258</v>
+      </c>
+      <c r="K2">
+        <v>160</v>
+      </c>
+      <c r="L2" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="M2">
+        <v>96</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>